<commit_message>
update feedback template resource with new version
</commit_message>
<xml_diff>
--- a/assets/resources/outcomes-feedback-template.xlsx
+++ b/assets/resources/outcomes-feedback-template.xlsx
@@ -12,7 +12,7 @@
     <definedName name="CodeList">Codes!$B$3:$B$27</definedName>
     <definedName name="Codes">Codes!$B$3:$C$11</definedName>
     <definedName name="OutcomeCodesRequiringPermission">Codes!$B$31:$B$53</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Template!$A$1:$U$1</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Template!$A$1:$Z$1</definedName>
     <definedName hidden="1" localSheetId="2" name="_xlnm._FilterDatabase">Codes!$B$30:$D$30</definedName>
   </definedNames>
   <calcPr/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="212">
   <si>
     <t>Feedback to the shielded vulnerable people service.</t>
   </si>
@@ -162,6 +162,21 @@
     <t>OutcomeComments</t>
   </si>
   <si>
+    <t>UPRN</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Mobile</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>LAPriority</t>
+  </si>
+  <si>
     <t>Description</t>
   </si>
   <si>
@@ -181,7 +196,7 @@
   </si>
   <si>
     <t>Wholesaler to continue food box delivery 
-(optional access free text. Max 200 characters)</t>
+(optional access free text. Max 125 characters)</t>
   </si>
   <si>
     <t>CC001</t>
@@ -648,6 +663,12 @@
   </si>
   <si>
     <t>Addition of Version Control.  Release for mainstream LAs.  Addition of comments validation - len 125</t>
+  </si>
+  <si>
+    <t>v0.12</t>
+  </si>
+  <si>
+    <t>Addition of New columns to match the latest output file</t>
   </si>
 </sst>
 </file>
@@ -657,7 +678,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="12.0"/>
       <color theme="1"/>
@@ -715,6 +736,11 @@
       <b/>
       <sz val="12.0"/>
       <color theme="0"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12.0"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -884,7 +910,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -919,10 +945,16 @@
     <xf borderId="12" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
+    <xf borderId="12" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
     <xf borderId="12" fillId="7" fontId="9" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="12" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="12" fillId="8" fontId="10" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
     <xf borderId="12" fillId="0" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="12" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -3043,6 +3075,21 @@
       <c r="U1" s="20" t="s">
         <v>42</v>
       </c>
+      <c r="V1" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="W1" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="X1" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y1" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z1" s="20" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="14"/>
@@ -3066,6 +3113,11 @@
       <c r="S2" s="23"/>
       <c r="T2" s="23"/>
       <c r="U2" s="23"/>
+      <c r="V2" s="23"/>
+      <c r="W2" s="23"/>
+      <c r="X2" s="23"/>
+      <c r="Y2" s="23"/>
+      <c r="Z2" s="23"/>
     </row>
     <row r="3">
       <c r="A3" s="14"/>
@@ -3089,6 +3141,11 @@
       <c r="S3" s="23"/>
       <c r="T3" s="23"/>
       <c r="U3" s="23"/>
+      <c r="V3" s="23"/>
+      <c r="W3" s="23"/>
+      <c r="X3" s="23"/>
+      <c r="Y3" s="23"/>
+      <c r="Z3" s="23"/>
     </row>
     <row r="4">
       <c r="A4" s="14"/>
@@ -3112,6 +3169,11 @@
       <c r="S4" s="23"/>
       <c r="T4" s="23"/>
       <c r="U4" s="23"/>
+      <c r="V4" s="23"/>
+      <c r="W4" s="23"/>
+      <c r="X4" s="23"/>
+      <c r="Y4" s="23"/>
+      <c r="Z4" s="23"/>
     </row>
     <row r="5">
       <c r="A5" s="14"/>
@@ -3135,6 +3197,11 @@
       <c r="S5" s="23"/>
       <c r="T5" s="23"/>
       <c r="U5" s="23"/>
+      <c r="V5" s="23"/>
+      <c r="W5" s="23"/>
+      <c r="X5" s="23"/>
+      <c r="Y5" s="23"/>
+      <c r="Z5" s="23"/>
     </row>
     <row r="6">
       <c r="A6" s="14"/>
@@ -3158,6 +3225,11 @@
       <c r="S6" s="23"/>
       <c r="T6" s="23"/>
       <c r="U6" s="23"/>
+      <c r="V6" s="23"/>
+      <c r="W6" s="23"/>
+      <c r="X6" s="23"/>
+      <c r="Y6" s="23"/>
+      <c r="Z6" s="23"/>
     </row>
     <row r="7">
       <c r="A7" s="14"/>
@@ -3181,6 +3253,11 @@
       <c r="S7" s="23"/>
       <c r="T7" s="23"/>
       <c r="U7" s="23"/>
+      <c r="V7" s="23"/>
+      <c r="W7" s="23"/>
+      <c r="X7" s="23"/>
+      <c r="Y7" s="23"/>
+      <c r="Z7" s="23"/>
     </row>
     <row r="8">
       <c r="A8" s="14"/>
@@ -3204,6 +3281,11 @@
       <c r="S8" s="23"/>
       <c r="T8" s="23"/>
       <c r="U8" s="23"/>
+      <c r="V8" s="23"/>
+      <c r="W8" s="23"/>
+      <c r="X8" s="23"/>
+      <c r="Y8" s="23"/>
+      <c r="Z8" s="23"/>
     </row>
     <row r="9">
       <c r="A9" s="14"/>
@@ -3227,6 +3309,11 @@
       <c r="S9" s="23"/>
       <c r="T9" s="23"/>
       <c r="U9" s="23"/>
+      <c r="V9" s="23"/>
+      <c r="W9" s="23"/>
+      <c r="X9" s="23"/>
+      <c r="Y9" s="23"/>
+      <c r="Z9" s="23"/>
     </row>
     <row r="10">
       <c r="A10" s="14"/>
@@ -3250,6 +3337,11 @@
       <c r="S10" s="23"/>
       <c r="T10" s="23"/>
       <c r="U10" s="23"/>
+      <c r="V10" s="23"/>
+      <c r="W10" s="23"/>
+      <c r="X10" s="23"/>
+      <c r="Y10" s="23"/>
+      <c r="Z10" s="23"/>
     </row>
     <row r="11">
       <c r="A11" s="14"/>
@@ -3273,6 +3365,11 @@
       <c r="S11" s="23"/>
       <c r="T11" s="23"/>
       <c r="U11" s="23"/>
+      <c r="V11" s="23"/>
+      <c r="W11" s="23"/>
+      <c r="X11" s="23"/>
+      <c r="Y11" s="23"/>
+      <c r="Z11" s="23"/>
     </row>
     <row r="12">
       <c r="A12" s="14"/>
@@ -3296,6 +3393,11 @@
       <c r="S12" s="23"/>
       <c r="T12" s="23"/>
       <c r="U12" s="23"/>
+      <c r="V12" s="23"/>
+      <c r="W12" s="23"/>
+      <c r="X12" s="23"/>
+      <c r="Y12" s="23"/>
+      <c r="Z12" s="23"/>
     </row>
     <row r="13">
       <c r="A13" s="14"/>
@@ -3319,6 +3421,11 @@
       <c r="S13" s="23"/>
       <c r="T13" s="23"/>
       <c r="U13" s="23"/>
+      <c r="V13" s="23"/>
+      <c r="W13" s="23"/>
+      <c r="X13" s="23"/>
+      <c r="Y13" s="23"/>
+      <c r="Z13" s="23"/>
     </row>
     <row r="14">
       <c r="A14" s="14"/>
@@ -3342,6 +3449,11 @@
       <c r="S14" s="23"/>
       <c r="T14" s="23"/>
       <c r="U14" s="23"/>
+      <c r="V14" s="23"/>
+      <c r="W14" s="23"/>
+      <c r="X14" s="23"/>
+      <c r="Y14" s="23"/>
+      <c r="Z14" s="23"/>
     </row>
     <row r="15">
       <c r="A15" s="14"/>
@@ -3365,6 +3477,11 @@
       <c r="S15" s="23"/>
       <c r="T15" s="23"/>
       <c r="U15" s="23"/>
+      <c r="V15" s="23"/>
+      <c r="W15" s="23"/>
+      <c r="X15" s="23"/>
+      <c r="Y15" s="23"/>
+      <c r="Z15" s="23"/>
     </row>
     <row r="16">
       <c r="A16" s="14"/>
@@ -3388,6 +3505,11 @@
       <c r="S16" s="23"/>
       <c r="T16" s="23"/>
       <c r="U16" s="23"/>
+      <c r="V16" s="23"/>
+      <c r="W16" s="23"/>
+      <c r="X16" s="23"/>
+      <c r="Y16" s="23"/>
+      <c r="Z16" s="23"/>
     </row>
     <row r="17">
       <c r="A17" s="14"/>
@@ -3411,6 +3533,11 @@
       <c r="S17" s="23"/>
       <c r="T17" s="23"/>
       <c r="U17" s="23"/>
+      <c r="V17" s="23"/>
+      <c r="W17" s="23"/>
+      <c r="X17" s="23"/>
+      <c r="Y17" s="23"/>
+      <c r="Z17" s="23"/>
     </row>
     <row r="18">
       <c r="A18" s="14"/>
@@ -3434,6 +3561,11 @@
       <c r="S18" s="23"/>
       <c r="T18" s="23"/>
       <c r="U18" s="23"/>
+      <c r="V18" s="23"/>
+      <c r="W18" s="23"/>
+      <c r="X18" s="23"/>
+      <c r="Y18" s="23"/>
+      <c r="Z18" s="23"/>
     </row>
     <row r="19">
       <c r="A19" s="14"/>
@@ -3457,6 +3589,11 @@
       <c r="S19" s="23"/>
       <c r="T19" s="23"/>
       <c r="U19" s="23"/>
+      <c r="V19" s="23"/>
+      <c r="W19" s="23"/>
+      <c r="X19" s="23"/>
+      <c r="Y19" s="23"/>
+      <c r="Z19" s="23"/>
     </row>
     <row r="20">
       <c r="A20" s="14"/>
@@ -3480,6 +3617,11 @@
       <c r="S20" s="23"/>
       <c r="T20" s="23"/>
       <c r="U20" s="23"/>
+      <c r="V20" s="23"/>
+      <c r="W20" s="23"/>
+      <c r="X20" s="23"/>
+      <c r="Y20" s="23"/>
+      <c r="Z20" s="23"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="14"/>
@@ -3503,6 +3645,11 @@
       <c r="S21" s="23"/>
       <c r="T21" s="23"/>
       <c r="U21" s="23"/>
+      <c r="V21" s="23"/>
+      <c r="W21" s="23"/>
+      <c r="X21" s="23"/>
+      <c r="Y21" s="23"/>
+      <c r="Z21" s="23"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="14"/>
@@ -3526,6 +3673,11 @@
       <c r="S22" s="23"/>
       <c r="T22" s="23"/>
       <c r="U22" s="23"/>
+      <c r="V22" s="23"/>
+      <c r="W22" s="23"/>
+      <c r="X22" s="23"/>
+      <c r="Y22" s="23"/>
+      <c r="Z22" s="23"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="14"/>
@@ -3549,6 +3701,11 @@
       <c r="S23" s="23"/>
       <c r="T23" s="23"/>
       <c r="U23" s="23"/>
+      <c r="V23" s="23"/>
+      <c r="W23" s="23"/>
+      <c r="X23" s="23"/>
+      <c r="Y23" s="23"/>
+      <c r="Z23" s="23"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="14"/>
@@ -3572,6 +3729,11 @@
       <c r="S24" s="23"/>
       <c r="T24" s="23"/>
       <c r="U24" s="23"/>
+      <c r="V24" s="23"/>
+      <c r="W24" s="23"/>
+      <c r="X24" s="23"/>
+      <c r="Y24" s="23"/>
+      <c r="Z24" s="23"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="14"/>
@@ -3595,6 +3757,11 @@
       <c r="S25" s="23"/>
       <c r="T25" s="23"/>
       <c r="U25" s="23"/>
+      <c r="V25" s="23"/>
+      <c r="W25" s="23"/>
+      <c r="X25" s="23"/>
+      <c r="Y25" s="23"/>
+      <c r="Z25" s="23"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="14"/>
@@ -3618,6 +3785,11 @@
       <c r="S26" s="23"/>
       <c r="T26" s="23"/>
       <c r="U26" s="23"/>
+      <c r="V26" s="23"/>
+      <c r="W26" s="23"/>
+      <c r="X26" s="23"/>
+      <c r="Y26" s="23"/>
+      <c r="Z26" s="23"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="14"/>
@@ -3641,6 +3813,11 @@
       <c r="S27" s="23"/>
       <c r="T27" s="23"/>
       <c r="U27" s="23"/>
+      <c r="V27" s="23"/>
+      <c r="W27" s="23"/>
+      <c r="X27" s="23"/>
+      <c r="Y27" s="23"/>
+      <c r="Z27" s="23"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="14"/>
@@ -3664,6 +3841,11 @@
       <c r="S28" s="23"/>
       <c r="T28" s="23"/>
       <c r="U28" s="23"/>
+      <c r="V28" s="23"/>
+      <c r="W28" s="23"/>
+      <c r="X28" s="23"/>
+      <c r="Y28" s="23"/>
+      <c r="Z28" s="23"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="14"/>
@@ -3687,6 +3869,11 @@
       <c r="S29" s="23"/>
       <c r="T29" s="23"/>
       <c r="U29" s="23"/>
+      <c r="V29" s="23"/>
+      <c r="W29" s="23"/>
+      <c r="X29" s="23"/>
+      <c r="Y29" s="23"/>
+      <c r="Z29" s="23"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="14"/>
@@ -3710,6 +3897,11 @@
       <c r="S30" s="23"/>
       <c r="T30" s="23"/>
       <c r="U30" s="23"/>
+      <c r="V30" s="23"/>
+      <c r="W30" s="23"/>
+      <c r="X30" s="23"/>
+      <c r="Y30" s="23"/>
+      <c r="Z30" s="23"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="14"/>
@@ -3733,6 +3925,11 @@
       <c r="S31" s="23"/>
       <c r="T31" s="23"/>
       <c r="U31" s="23"/>
+      <c r="V31" s="23"/>
+      <c r="W31" s="23"/>
+      <c r="X31" s="23"/>
+      <c r="Y31" s="23"/>
+      <c r="Z31" s="23"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="14"/>
@@ -3756,6 +3953,11 @@
       <c r="S32" s="23"/>
       <c r="T32" s="23"/>
       <c r="U32" s="23"/>
+      <c r="V32" s="23"/>
+      <c r="W32" s="23"/>
+      <c r="X32" s="23"/>
+      <c r="Y32" s="23"/>
+      <c r="Z32" s="23"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="14"/>
@@ -3779,6 +3981,11 @@
       <c r="S33" s="23"/>
       <c r="T33" s="23"/>
       <c r="U33" s="23"/>
+      <c r="V33" s="23"/>
+      <c r="W33" s="23"/>
+      <c r="X33" s="23"/>
+      <c r="Y33" s="23"/>
+      <c r="Z33" s="23"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="14"/>
@@ -3802,6 +4009,11 @@
       <c r="S34" s="23"/>
       <c r="T34" s="23"/>
       <c r="U34" s="23"/>
+      <c r="V34" s="23"/>
+      <c r="W34" s="23"/>
+      <c r="X34" s="23"/>
+      <c r="Y34" s="23"/>
+      <c r="Z34" s="23"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="14"/>
@@ -3825,6 +4037,11 @@
       <c r="S35" s="23"/>
       <c r="T35" s="23"/>
       <c r="U35" s="23"/>
+      <c r="V35" s="23"/>
+      <c r="W35" s="23"/>
+      <c r="X35" s="23"/>
+      <c r="Y35" s="23"/>
+      <c r="Z35" s="23"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="14"/>
@@ -3848,6 +4065,11 @@
       <c r="S36" s="23"/>
       <c r="T36" s="23"/>
       <c r="U36" s="23"/>
+      <c r="V36" s="23"/>
+      <c r="W36" s="23"/>
+      <c r="X36" s="23"/>
+      <c r="Y36" s="23"/>
+      <c r="Z36" s="23"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="14"/>
@@ -3871,6 +4093,11 @@
       <c r="S37" s="23"/>
       <c r="T37" s="23"/>
       <c r="U37" s="23"/>
+      <c r="V37" s="23"/>
+      <c r="W37" s="23"/>
+      <c r="X37" s="23"/>
+      <c r="Y37" s="23"/>
+      <c r="Z37" s="23"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="14"/>
@@ -3894,6 +4121,11 @@
       <c r="S38" s="23"/>
       <c r="T38" s="23"/>
       <c r="U38" s="23"/>
+      <c r="V38" s="23"/>
+      <c r="W38" s="23"/>
+      <c r="X38" s="23"/>
+      <c r="Y38" s="23"/>
+      <c r="Z38" s="23"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="14"/>
@@ -3917,6 +4149,11 @@
       <c r="S39" s="23"/>
       <c r="T39" s="23"/>
       <c r="U39" s="23"/>
+      <c r="V39" s="23"/>
+      <c r="W39" s="23"/>
+      <c r="X39" s="23"/>
+      <c r="Y39" s="23"/>
+      <c r="Z39" s="23"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="14"/>
@@ -3940,6 +4177,11 @@
       <c r="S40" s="23"/>
       <c r="T40" s="23"/>
       <c r="U40" s="23"/>
+      <c r="V40" s="23"/>
+      <c r="W40" s="23"/>
+      <c r="X40" s="23"/>
+      <c r="Y40" s="23"/>
+      <c r="Z40" s="23"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="14"/>
@@ -3963,6 +4205,11 @@
       <c r="S41" s="23"/>
       <c r="T41" s="23"/>
       <c r="U41" s="23"/>
+      <c r="V41" s="23"/>
+      <c r="W41" s="23"/>
+      <c r="X41" s="23"/>
+      <c r="Y41" s="23"/>
+      <c r="Z41" s="23"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="14"/>
@@ -3986,6 +4233,11 @@
       <c r="S42" s="23"/>
       <c r="T42" s="23"/>
       <c r="U42" s="23"/>
+      <c r="V42" s="23"/>
+      <c r="W42" s="23"/>
+      <c r="X42" s="23"/>
+      <c r="Y42" s="23"/>
+      <c r="Z42" s="23"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="14"/>
@@ -4009,6 +4261,11 @@
       <c r="S43" s="23"/>
       <c r="T43" s="23"/>
       <c r="U43" s="23"/>
+      <c r="V43" s="23"/>
+      <c r="W43" s="23"/>
+      <c r="X43" s="23"/>
+      <c r="Y43" s="23"/>
+      <c r="Z43" s="23"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="14"/>
@@ -4032,6 +4289,11 @@
       <c r="S44" s="23"/>
       <c r="T44" s="23"/>
       <c r="U44" s="23"/>
+      <c r="V44" s="23"/>
+      <c r="W44" s="23"/>
+      <c r="X44" s="23"/>
+      <c r="Y44" s="23"/>
+      <c r="Z44" s="23"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="14"/>
@@ -4055,6 +4317,11 @@
       <c r="S45" s="23"/>
       <c r="T45" s="23"/>
       <c r="U45" s="23"/>
+      <c r="V45" s="23"/>
+      <c r="W45" s="23"/>
+      <c r="X45" s="23"/>
+      <c r="Y45" s="23"/>
+      <c r="Z45" s="23"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="14"/>
@@ -4078,6 +4345,11 @@
       <c r="S46" s="23"/>
       <c r="T46" s="23"/>
       <c r="U46" s="23"/>
+      <c r="V46" s="23"/>
+      <c r="W46" s="23"/>
+      <c r="X46" s="23"/>
+      <c r="Y46" s="23"/>
+      <c r="Z46" s="23"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
       <c r="A47" s="14"/>
@@ -4101,6 +4373,11 @@
       <c r="S47" s="23"/>
       <c r="T47" s="23"/>
       <c r="U47" s="23"/>
+      <c r="V47" s="23"/>
+      <c r="W47" s="23"/>
+      <c r="X47" s="23"/>
+      <c r="Y47" s="23"/>
+      <c r="Z47" s="23"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="14"/>
@@ -4124,6 +4401,11 @@
       <c r="S48" s="23"/>
       <c r="T48" s="23"/>
       <c r="U48" s="23"/>
+      <c r="V48" s="23"/>
+      <c r="W48" s="23"/>
+      <c r="X48" s="23"/>
+      <c r="Y48" s="23"/>
+      <c r="Z48" s="23"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="14"/>
@@ -4147,6 +4429,11 @@
       <c r="S49" s="23"/>
       <c r="T49" s="23"/>
       <c r="U49" s="23"/>
+      <c r="V49" s="23"/>
+      <c r="W49" s="23"/>
+      <c r="X49" s="23"/>
+      <c r="Y49" s="23"/>
+      <c r="Z49" s="23"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
       <c r="A50" s="14"/>
@@ -4170,6 +4457,11 @@
       <c r="S50" s="23"/>
       <c r="T50" s="23"/>
       <c r="U50" s="23"/>
+      <c r="V50" s="23"/>
+      <c r="W50" s="23"/>
+      <c r="X50" s="23"/>
+      <c r="Y50" s="23"/>
+      <c r="Z50" s="23"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
       <c r="A51" s="14"/>
@@ -4193,6 +4485,11 @@
       <c r="S51" s="23"/>
       <c r="T51" s="23"/>
       <c r="U51" s="23"/>
+      <c r="V51" s="23"/>
+      <c r="W51" s="23"/>
+      <c r="X51" s="23"/>
+      <c r="Y51" s="23"/>
+      <c r="Z51" s="23"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" s="14"/>
@@ -4216,6 +4513,11 @@
       <c r="S52" s="23"/>
       <c r="T52" s="23"/>
       <c r="U52" s="23"/>
+      <c r="V52" s="23"/>
+      <c r="W52" s="23"/>
+      <c r="X52" s="23"/>
+      <c r="Y52" s="23"/>
+      <c r="Z52" s="23"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="A53" s="14"/>
@@ -4239,6 +4541,11 @@
       <c r="S53" s="23"/>
       <c r="T53" s="23"/>
       <c r="U53" s="23"/>
+      <c r="V53" s="23"/>
+      <c r="W53" s="23"/>
+      <c r="X53" s="23"/>
+      <c r="Y53" s="23"/>
+      <c r="Z53" s="23"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
       <c r="A54" s="14"/>
@@ -4262,6 +4569,11 @@
       <c r="S54" s="23"/>
       <c r="T54" s="23"/>
       <c r="U54" s="23"/>
+      <c r="V54" s="23"/>
+      <c r="W54" s="23"/>
+      <c r="X54" s="23"/>
+      <c r="Y54" s="23"/>
+      <c r="Z54" s="23"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
       <c r="A55" s="14"/>
@@ -4285,6 +4597,11 @@
       <c r="S55" s="23"/>
       <c r="T55" s="23"/>
       <c r="U55" s="23"/>
+      <c r="V55" s="23"/>
+      <c r="W55" s="23"/>
+      <c r="X55" s="23"/>
+      <c r="Y55" s="23"/>
+      <c r="Z55" s="23"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
       <c r="A56" s="14"/>
@@ -4308,6 +4625,11 @@
       <c r="S56" s="23"/>
       <c r="T56" s="23"/>
       <c r="U56" s="23"/>
+      <c r="V56" s="23"/>
+      <c r="W56" s="23"/>
+      <c r="X56" s="23"/>
+      <c r="Y56" s="23"/>
+      <c r="Z56" s="23"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
       <c r="A57" s="14"/>
@@ -4331,6 +4653,11 @@
       <c r="S57" s="23"/>
       <c r="T57" s="23"/>
       <c r="U57" s="23"/>
+      <c r="V57" s="23"/>
+      <c r="W57" s="23"/>
+      <c r="X57" s="23"/>
+      <c r="Y57" s="23"/>
+      <c r="Z57" s="23"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="14"/>
@@ -4354,6 +4681,11 @@
       <c r="S58" s="23"/>
       <c r="T58" s="23"/>
       <c r="U58" s="23"/>
+      <c r="V58" s="23"/>
+      <c r="W58" s="23"/>
+      <c r="X58" s="23"/>
+      <c r="Y58" s="23"/>
+      <c r="Z58" s="23"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
       <c r="A59" s="14"/>
@@ -4377,6 +4709,11 @@
       <c r="S59" s="23"/>
       <c r="T59" s="23"/>
       <c r="U59" s="23"/>
+      <c r="V59" s="23"/>
+      <c r="W59" s="23"/>
+      <c r="X59" s="23"/>
+      <c r="Y59" s="23"/>
+      <c r="Z59" s="23"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
       <c r="A60" s="14"/>
@@ -4400,6 +4737,11 @@
       <c r="S60" s="23"/>
       <c r="T60" s="23"/>
       <c r="U60" s="23"/>
+      <c r="V60" s="23"/>
+      <c r="W60" s="23"/>
+      <c r="X60" s="23"/>
+      <c r="Y60" s="23"/>
+      <c r="Z60" s="23"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
       <c r="A61" s="14"/>
@@ -4423,6 +4765,11 @@
       <c r="S61" s="23"/>
       <c r="T61" s="23"/>
       <c r="U61" s="23"/>
+      <c r="V61" s="23"/>
+      <c r="W61" s="23"/>
+      <c r="X61" s="23"/>
+      <c r="Y61" s="23"/>
+      <c r="Z61" s="23"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
       <c r="A62" s="14"/>
@@ -4446,6 +4793,11 @@
       <c r="S62" s="23"/>
       <c r="T62" s="23"/>
       <c r="U62" s="23"/>
+      <c r="V62" s="23"/>
+      <c r="W62" s="23"/>
+      <c r="X62" s="23"/>
+      <c r="Y62" s="23"/>
+      <c r="Z62" s="23"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
       <c r="A63" s="14"/>
@@ -4469,6 +4821,11 @@
       <c r="S63" s="23"/>
       <c r="T63" s="23"/>
       <c r="U63" s="23"/>
+      <c r="V63" s="23"/>
+      <c r="W63" s="23"/>
+      <c r="X63" s="23"/>
+      <c r="Y63" s="23"/>
+      <c r="Z63" s="23"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
       <c r="A64" s="14"/>
@@ -4492,6 +4849,11 @@
       <c r="S64" s="23"/>
       <c r="T64" s="23"/>
       <c r="U64" s="23"/>
+      <c r="V64" s="23"/>
+      <c r="W64" s="23"/>
+      <c r="X64" s="23"/>
+      <c r="Y64" s="23"/>
+      <c r="Z64" s="23"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
       <c r="A65" s="14"/>
@@ -4515,6 +4877,11 @@
       <c r="S65" s="23"/>
       <c r="T65" s="23"/>
       <c r="U65" s="23"/>
+      <c r="V65" s="23"/>
+      <c r="W65" s="23"/>
+      <c r="X65" s="23"/>
+      <c r="Y65" s="23"/>
+      <c r="Z65" s="23"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
       <c r="A66" s="14"/>
@@ -4538,6 +4905,11 @@
       <c r="S66" s="23"/>
       <c r="T66" s="23"/>
       <c r="U66" s="23"/>
+      <c r="V66" s="23"/>
+      <c r="W66" s="23"/>
+      <c r="X66" s="23"/>
+      <c r="Y66" s="23"/>
+      <c r="Z66" s="23"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
       <c r="A67" s="14"/>
@@ -4561,6 +4933,11 @@
       <c r="S67" s="23"/>
       <c r="T67" s="23"/>
       <c r="U67" s="23"/>
+      <c r="V67" s="23"/>
+      <c r="W67" s="23"/>
+      <c r="X67" s="23"/>
+      <c r="Y67" s="23"/>
+      <c r="Z67" s="23"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
       <c r="A68" s="14"/>
@@ -4584,6 +4961,11 @@
       <c r="S68" s="23"/>
       <c r="T68" s="23"/>
       <c r="U68" s="23"/>
+      <c r="V68" s="23"/>
+      <c r="W68" s="23"/>
+      <c r="X68" s="23"/>
+      <c r="Y68" s="23"/>
+      <c r="Z68" s="23"/>
     </row>
     <row r="69" ht="15.75" customHeight="1">
       <c r="A69" s="14"/>
@@ -4607,6 +4989,11 @@
       <c r="S69" s="23"/>
       <c r="T69" s="23"/>
       <c r="U69" s="23"/>
+      <c r="V69" s="23"/>
+      <c r="W69" s="23"/>
+      <c r="X69" s="23"/>
+      <c r="Y69" s="23"/>
+      <c r="Z69" s="23"/>
     </row>
     <row r="70" ht="15.75" customHeight="1">
       <c r="A70" s="14"/>
@@ -4630,6 +5017,11 @@
       <c r="S70" s="23"/>
       <c r="T70" s="23"/>
       <c r="U70" s="23"/>
+      <c r="V70" s="23"/>
+      <c r="W70" s="23"/>
+      <c r="X70" s="23"/>
+      <c r="Y70" s="23"/>
+      <c r="Z70" s="23"/>
     </row>
     <row r="71" ht="15.75" customHeight="1">
       <c r="A71" s="14"/>
@@ -4653,6 +5045,11 @@
       <c r="S71" s="23"/>
       <c r="T71" s="23"/>
       <c r="U71" s="23"/>
+      <c r="V71" s="23"/>
+      <c r="W71" s="23"/>
+      <c r="X71" s="23"/>
+      <c r="Y71" s="23"/>
+      <c r="Z71" s="23"/>
     </row>
     <row r="72" ht="15.75" customHeight="1">
       <c r="A72" s="14"/>
@@ -4676,6 +5073,11 @@
       <c r="S72" s="23"/>
       <c r="T72" s="23"/>
       <c r="U72" s="23"/>
+      <c r="V72" s="23"/>
+      <c r="W72" s="23"/>
+      <c r="X72" s="23"/>
+      <c r="Y72" s="23"/>
+      <c r="Z72" s="23"/>
     </row>
     <row r="73" ht="15.75" customHeight="1">
       <c r="A73" s="14"/>
@@ -4699,6 +5101,11 @@
       <c r="S73" s="23"/>
       <c r="T73" s="23"/>
       <c r="U73" s="23"/>
+      <c r="V73" s="23"/>
+      <c r="W73" s="23"/>
+      <c r="X73" s="23"/>
+      <c r="Y73" s="23"/>
+      <c r="Z73" s="23"/>
     </row>
     <row r="74" ht="15.75" customHeight="1">
       <c r="A74" s="14"/>
@@ -4722,6 +5129,11 @@
       <c r="S74" s="23"/>
       <c r="T74" s="23"/>
       <c r="U74" s="23"/>
+      <c r="V74" s="23"/>
+      <c r="W74" s="23"/>
+      <c r="X74" s="23"/>
+      <c r="Y74" s="23"/>
+      <c r="Z74" s="23"/>
     </row>
     <row r="75" ht="15.75" customHeight="1">
       <c r="A75" s="14"/>
@@ -4745,6 +5157,11 @@
       <c r="S75" s="23"/>
       <c r="T75" s="23"/>
       <c r="U75" s="23"/>
+      <c r="V75" s="23"/>
+      <c r="W75" s="23"/>
+      <c r="X75" s="23"/>
+      <c r="Y75" s="23"/>
+      <c r="Z75" s="23"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
       <c r="A76" s="14"/>
@@ -4768,6 +5185,11 @@
       <c r="S76" s="23"/>
       <c r="T76" s="23"/>
       <c r="U76" s="23"/>
+      <c r="V76" s="23"/>
+      <c r="W76" s="23"/>
+      <c r="X76" s="23"/>
+      <c r="Y76" s="23"/>
+      <c r="Z76" s="23"/>
     </row>
     <row r="77" ht="15.75" customHeight="1">
       <c r="A77" s="14"/>
@@ -4791,6 +5213,11 @@
       <c r="S77" s="23"/>
       <c r="T77" s="23"/>
       <c r="U77" s="23"/>
+      <c r="V77" s="23"/>
+      <c r="W77" s="23"/>
+      <c r="X77" s="23"/>
+      <c r="Y77" s="23"/>
+      <c r="Z77" s="23"/>
     </row>
     <row r="78" ht="15.75" customHeight="1">
       <c r="A78" s="14"/>
@@ -4814,6 +5241,11 @@
       <c r="S78" s="23"/>
       <c r="T78" s="23"/>
       <c r="U78" s="23"/>
+      <c r="V78" s="23"/>
+      <c r="W78" s="23"/>
+      <c r="X78" s="23"/>
+      <c r="Y78" s="23"/>
+      <c r="Z78" s="23"/>
     </row>
     <row r="79" ht="15.75" customHeight="1">
       <c r="A79" s="14"/>
@@ -4837,6 +5269,11 @@
       <c r="S79" s="23"/>
       <c r="T79" s="23"/>
       <c r="U79" s="23"/>
+      <c r="V79" s="23"/>
+      <c r="W79" s="23"/>
+      <c r="X79" s="23"/>
+      <c r="Y79" s="23"/>
+      <c r="Z79" s="23"/>
     </row>
     <row r="80" ht="15.75" customHeight="1">
       <c r="A80" s="14"/>
@@ -4860,6 +5297,11 @@
       <c r="S80" s="23"/>
       <c r="T80" s="23"/>
       <c r="U80" s="23"/>
+      <c r="V80" s="23"/>
+      <c r="W80" s="23"/>
+      <c r="X80" s="23"/>
+      <c r="Y80" s="23"/>
+      <c r="Z80" s="23"/>
     </row>
     <row r="81" ht="15.75" customHeight="1">
       <c r="A81" s="14"/>
@@ -4883,6 +5325,11 @@
       <c r="S81" s="23"/>
       <c r="T81" s="23"/>
       <c r="U81" s="23"/>
+      <c r="V81" s="23"/>
+      <c r="W81" s="23"/>
+      <c r="X81" s="23"/>
+      <c r="Y81" s="23"/>
+      <c r="Z81" s="23"/>
     </row>
     <row r="82" ht="15.75" customHeight="1">
       <c r="A82" s="14"/>
@@ -4906,6 +5353,11 @@
       <c r="S82" s="23"/>
       <c r="T82" s="23"/>
       <c r="U82" s="23"/>
+      <c r="V82" s="23"/>
+      <c r="W82" s="23"/>
+      <c r="X82" s="23"/>
+      <c r="Y82" s="23"/>
+      <c r="Z82" s="23"/>
     </row>
     <row r="83" ht="15.75" customHeight="1">
       <c r="A83" s="14"/>
@@ -4929,6 +5381,11 @@
       <c r="S83" s="23"/>
       <c r="T83" s="23"/>
       <c r="U83" s="23"/>
+      <c r="V83" s="23"/>
+      <c r="W83" s="23"/>
+      <c r="X83" s="23"/>
+      <c r="Y83" s="23"/>
+      <c r="Z83" s="23"/>
     </row>
     <row r="84" ht="15.75" customHeight="1">
       <c r="A84" s="14"/>
@@ -4952,6 +5409,11 @@
       <c r="S84" s="23"/>
       <c r="T84" s="23"/>
       <c r="U84" s="23"/>
+      <c r="V84" s="23"/>
+      <c r="W84" s="23"/>
+      <c r="X84" s="23"/>
+      <c r="Y84" s="23"/>
+      <c r="Z84" s="23"/>
     </row>
     <row r="85" ht="15.75" customHeight="1">
       <c r="A85" s="14"/>
@@ -4975,6 +5437,11 @@
       <c r="S85" s="23"/>
       <c r="T85" s="23"/>
       <c r="U85" s="23"/>
+      <c r="V85" s="23"/>
+      <c r="W85" s="23"/>
+      <c r="X85" s="23"/>
+      <c r="Y85" s="23"/>
+      <c r="Z85" s="23"/>
     </row>
     <row r="86" ht="15.75" customHeight="1">
       <c r="A86" s="14"/>
@@ -4998,6 +5465,11 @@
       <c r="S86" s="23"/>
       <c r="T86" s="23"/>
       <c r="U86" s="23"/>
+      <c r="V86" s="23"/>
+      <c r="W86" s="23"/>
+      <c r="X86" s="23"/>
+      <c r="Y86" s="23"/>
+      <c r="Z86" s="23"/>
     </row>
     <row r="87" ht="15.75" customHeight="1">
       <c r="A87" s="14"/>
@@ -5021,6 +5493,11 @@
       <c r="S87" s="23"/>
       <c r="T87" s="23"/>
       <c r="U87" s="23"/>
+      <c r="V87" s="23"/>
+      <c r="W87" s="23"/>
+      <c r="X87" s="23"/>
+      <c r="Y87" s="23"/>
+      <c r="Z87" s="23"/>
     </row>
     <row r="88" ht="15.75" customHeight="1">
       <c r="A88" s="14"/>
@@ -5044,6 +5521,11 @@
       <c r="S88" s="23"/>
       <c r="T88" s="23"/>
       <c r="U88" s="23"/>
+      <c r="V88" s="23"/>
+      <c r="W88" s="23"/>
+      <c r="X88" s="23"/>
+      <c r="Y88" s="23"/>
+      <c r="Z88" s="23"/>
     </row>
     <row r="89" ht="15.75" customHeight="1">
       <c r="A89" s="14"/>
@@ -5067,6 +5549,11 @@
       <c r="S89" s="23"/>
       <c r="T89" s="23"/>
       <c r="U89" s="23"/>
+      <c r="V89" s="23"/>
+      <c r="W89" s="23"/>
+      <c r="X89" s="23"/>
+      <c r="Y89" s="23"/>
+      <c r="Z89" s="23"/>
     </row>
     <row r="90" ht="15.75" customHeight="1">
       <c r="A90" s="14"/>
@@ -5090,6 +5577,11 @@
       <c r="S90" s="23"/>
       <c r="T90" s="23"/>
       <c r="U90" s="23"/>
+      <c r="V90" s="23"/>
+      <c r="W90" s="23"/>
+      <c r="X90" s="23"/>
+      <c r="Y90" s="23"/>
+      <c r="Z90" s="23"/>
     </row>
     <row r="91" ht="15.75" customHeight="1">
       <c r="A91" s="14"/>
@@ -5113,6 +5605,11 @@
       <c r="S91" s="23"/>
       <c r="T91" s="23"/>
       <c r="U91" s="23"/>
+      <c r="V91" s="23"/>
+      <c r="W91" s="23"/>
+      <c r="X91" s="23"/>
+      <c r="Y91" s="23"/>
+      <c r="Z91" s="23"/>
     </row>
     <row r="92" ht="15.75" customHeight="1">
       <c r="A92" s="14"/>
@@ -5136,6 +5633,11 @@
       <c r="S92" s="23"/>
       <c r="T92" s="23"/>
       <c r="U92" s="23"/>
+      <c r="V92" s="23"/>
+      <c r="W92" s="23"/>
+      <c r="X92" s="23"/>
+      <c r="Y92" s="23"/>
+      <c r="Z92" s="23"/>
     </row>
     <row r="93" ht="15.75" customHeight="1">
       <c r="A93" s="14"/>
@@ -5159,6 +5661,11 @@
       <c r="S93" s="23"/>
       <c r="T93" s="23"/>
       <c r="U93" s="23"/>
+      <c r="V93" s="23"/>
+      <c r="W93" s="23"/>
+      <c r="X93" s="23"/>
+      <c r="Y93" s="23"/>
+      <c r="Z93" s="23"/>
     </row>
     <row r="94" ht="15.75" customHeight="1">
       <c r="A94" s="14"/>
@@ -5182,6 +5689,11 @@
       <c r="S94" s="23"/>
       <c r="T94" s="23"/>
       <c r="U94" s="23"/>
+      <c r="V94" s="23"/>
+      <c r="W94" s="23"/>
+      <c r="X94" s="23"/>
+      <c r="Y94" s="23"/>
+      <c r="Z94" s="23"/>
     </row>
     <row r="95" ht="15.75" customHeight="1">
       <c r="A95" s="14"/>
@@ -5205,6 +5717,11 @@
       <c r="S95" s="23"/>
       <c r="T95" s="23"/>
       <c r="U95" s="23"/>
+      <c r="V95" s="23"/>
+      <c r="W95" s="23"/>
+      <c r="X95" s="23"/>
+      <c r="Y95" s="23"/>
+      <c r="Z95" s="23"/>
     </row>
     <row r="96" ht="15.75" customHeight="1">
       <c r="A96" s="14"/>
@@ -5228,6 +5745,11 @@
       <c r="S96" s="23"/>
       <c r="T96" s="23"/>
       <c r="U96" s="23"/>
+      <c r="V96" s="23"/>
+      <c r="W96" s="23"/>
+      <c r="X96" s="23"/>
+      <c r="Y96" s="23"/>
+      <c r="Z96" s="23"/>
     </row>
     <row r="97" ht="15.75" customHeight="1">
       <c r="A97" s="14"/>
@@ -5251,6 +5773,11 @@
       <c r="S97" s="23"/>
       <c r="T97" s="23"/>
       <c r="U97" s="23"/>
+      <c r="V97" s="23"/>
+      <c r="W97" s="23"/>
+      <c r="X97" s="23"/>
+      <c r="Y97" s="23"/>
+      <c r="Z97" s="23"/>
     </row>
     <row r="98" ht="15.75" customHeight="1">
       <c r="A98" s="14"/>
@@ -5274,6 +5801,11 @@
       <c r="S98" s="23"/>
       <c r="T98" s="23"/>
       <c r="U98" s="23"/>
+      <c r="V98" s="23"/>
+      <c r="W98" s="23"/>
+      <c r="X98" s="23"/>
+      <c r="Y98" s="23"/>
+      <c r="Z98" s="23"/>
     </row>
     <row r="99" ht="15.75" customHeight="1">
       <c r="A99" s="14"/>
@@ -5297,6 +5829,11 @@
       <c r="S99" s="23"/>
       <c r="T99" s="23"/>
       <c r="U99" s="23"/>
+      <c r="V99" s="23"/>
+      <c r="W99" s="23"/>
+      <c r="X99" s="23"/>
+      <c r="Y99" s="23"/>
+      <c r="Z99" s="23"/>
     </row>
     <row r="100" ht="15.75" customHeight="1">
       <c r="A100" s="14"/>
@@ -5320,6 +5857,11 @@
       <c r="S100" s="23"/>
       <c r="T100" s="23"/>
       <c r="U100" s="23"/>
+      <c r="V100" s="23"/>
+      <c r="W100" s="23"/>
+      <c r="X100" s="23"/>
+      <c r="Y100" s="23"/>
+      <c r="Z100" s="23"/>
     </row>
     <row r="101" ht="15.75" customHeight="1">
       <c r="A101" s="14"/>
@@ -5343,6 +5885,11 @@
       <c r="S101" s="23"/>
       <c r="T101" s="23"/>
       <c r="U101" s="23"/>
+      <c r="V101" s="23"/>
+      <c r="W101" s="23"/>
+      <c r="X101" s="23"/>
+      <c r="Y101" s="23"/>
+      <c r="Z101" s="23"/>
     </row>
     <row r="102" ht="15.75" customHeight="1">
       <c r="A102" s="14"/>
@@ -5366,6 +5913,11 @@
       <c r="S102" s="23"/>
       <c r="T102" s="23"/>
       <c r="U102" s="23"/>
+      <c r="V102" s="23"/>
+      <c r="W102" s="23"/>
+      <c r="X102" s="23"/>
+      <c r="Y102" s="23"/>
+      <c r="Z102" s="23"/>
     </row>
     <row r="103" ht="15.75" customHeight="1">
       <c r="A103" s="14"/>
@@ -5389,6 +5941,11 @@
       <c r="S103" s="23"/>
       <c r="T103" s="23"/>
       <c r="U103" s="23"/>
+      <c r="V103" s="23"/>
+      <c r="W103" s="23"/>
+      <c r="X103" s="23"/>
+      <c r="Y103" s="23"/>
+      <c r="Z103" s="23"/>
     </row>
     <row r="104" ht="15.75" customHeight="1">
       <c r="A104" s="14"/>
@@ -5412,6 +5969,11 @@
       <c r="S104" s="23"/>
       <c r="T104" s="23"/>
       <c r="U104" s="23"/>
+      <c r="V104" s="23"/>
+      <c r="W104" s="23"/>
+      <c r="X104" s="23"/>
+      <c r="Y104" s="23"/>
+      <c r="Z104" s="23"/>
     </row>
     <row r="105" ht="15.75" customHeight="1">
       <c r="A105" s="14"/>
@@ -5435,6 +5997,11 @@
       <c r="S105" s="23"/>
       <c r="T105" s="23"/>
       <c r="U105" s="23"/>
+      <c r="V105" s="23"/>
+      <c r="W105" s="23"/>
+      <c r="X105" s="23"/>
+      <c r="Y105" s="23"/>
+      <c r="Z105" s="23"/>
     </row>
     <row r="106" ht="15.75" customHeight="1">
       <c r="A106" s="14"/>
@@ -5458,6 +6025,11 @@
       <c r="S106" s="23"/>
       <c r="T106" s="23"/>
       <c r="U106" s="23"/>
+      <c r="V106" s="23"/>
+      <c r="W106" s="23"/>
+      <c r="X106" s="23"/>
+      <c r="Y106" s="23"/>
+      <c r="Z106" s="23"/>
     </row>
     <row r="107" ht="15.75" customHeight="1">
       <c r="A107" s="14"/>
@@ -5481,6 +6053,11 @@
       <c r="S107" s="23"/>
       <c r="T107" s="23"/>
       <c r="U107" s="23"/>
+      <c r="V107" s="23"/>
+      <c r="W107" s="23"/>
+      <c r="X107" s="23"/>
+      <c r="Y107" s="23"/>
+      <c r="Z107" s="23"/>
     </row>
     <row r="108" ht="15.75" customHeight="1">
       <c r="A108" s="14"/>
@@ -5504,6 +6081,11 @@
       <c r="S108" s="23"/>
       <c r="T108" s="23"/>
       <c r="U108" s="23"/>
+      <c r="V108" s="23"/>
+      <c r="W108" s="23"/>
+      <c r="X108" s="23"/>
+      <c r="Y108" s="23"/>
+      <c r="Z108" s="23"/>
     </row>
     <row r="109" ht="15.75" customHeight="1">
       <c r="A109" s="14"/>
@@ -5527,6 +6109,11 @@
       <c r="S109" s="23"/>
       <c r="T109" s="23"/>
       <c r="U109" s="23"/>
+      <c r="V109" s="23"/>
+      <c r="W109" s="23"/>
+      <c r="X109" s="23"/>
+      <c r="Y109" s="23"/>
+      <c r="Z109" s="23"/>
     </row>
     <row r="110" ht="15.75" customHeight="1">
       <c r="A110" s="14"/>
@@ -5550,6 +6137,11 @@
       <c r="S110" s="23"/>
       <c r="T110" s="23"/>
       <c r="U110" s="23"/>
+      <c r="V110" s="23"/>
+      <c r="W110" s="23"/>
+      <c r="X110" s="23"/>
+      <c r="Y110" s="23"/>
+      <c r="Z110" s="23"/>
     </row>
     <row r="111" ht="15.75" customHeight="1">
       <c r="A111" s="14"/>
@@ -5573,6 +6165,11 @@
       <c r="S111" s="23"/>
       <c r="T111" s="23"/>
       <c r="U111" s="23"/>
+      <c r="V111" s="23"/>
+      <c r="W111" s="23"/>
+      <c r="X111" s="23"/>
+      <c r="Y111" s="23"/>
+      <c r="Z111" s="23"/>
     </row>
     <row r="112" ht="15.75" customHeight="1">
       <c r="A112" s="14"/>
@@ -5596,6 +6193,11 @@
       <c r="S112" s="23"/>
       <c r="T112" s="23"/>
       <c r="U112" s="23"/>
+      <c r="V112" s="23"/>
+      <c r="W112" s="23"/>
+      <c r="X112" s="23"/>
+      <c r="Y112" s="23"/>
+      <c r="Z112" s="23"/>
     </row>
     <row r="113" ht="15.75" customHeight="1">
       <c r="A113" s="14"/>
@@ -5619,6 +6221,11 @@
       <c r="S113" s="23"/>
       <c r="T113" s="23"/>
       <c r="U113" s="23"/>
+      <c r="V113" s="23"/>
+      <c r="W113" s="23"/>
+      <c r="X113" s="23"/>
+      <c r="Y113" s="23"/>
+      <c r="Z113" s="23"/>
     </row>
     <row r="114" ht="15.75" customHeight="1">
       <c r="A114" s="14"/>
@@ -5642,6 +6249,11 @@
       <c r="S114" s="23"/>
       <c r="T114" s="23"/>
       <c r="U114" s="23"/>
+      <c r="V114" s="23"/>
+      <c r="W114" s="23"/>
+      <c r="X114" s="23"/>
+      <c r="Y114" s="23"/>
+      <c r="Z114" s="23"/>
     </row>
     <row r="115" ht="15.75" customHeight="1">
       <c r="A115" s="14"/>
@@ -5665,6 +6277,11 @@
       <c r="S115" s="23"/>
       <c r="T115" s="23"/>
       <c r="U115" s="23"/>
+      <c r="V115" s="23"/>
+      <c r="W115" s="23"/>
+      <c r="X115" s="23"/>
+      <c r="Y115" s="23"/>
+      <c r="Z115" s="23"/>
     </row>
     <row r="116" ht="15.75" customHeight="1">
       <c r="A116" s="14"/>
@@ -5688,6 +6305,11 @@
       <c r="S116" s="23"/>
       <c r="T116" s="23"/>
       <c r="U116" s="23"/>
+      <c r="V116" s="23"/>
+      <c r="W116" s="23"/>
+      <c r="X116" s="23"/>
+      <c r="Y116" s="23"/>
+      <c r="Z116" s="23"/>
     </row>
     <row r="117" ht="15.75" customHeight="1">
       <c r="A117" s="14"/>
@@ -5711,6 +6333,11 @@
       <c r="S117" s="23"/>
       <c r="T117" s="23"/>
       <c r="U117" s="23"/>
+      <c r="V117" s="23"/>
+      <c r="W117" s="23"/>
+      <c r="X117" s="23"/>
+      <c r="Y117" s="23"/>
+      <c r="Z117" s="23"/>
     </row>
     <row r="118" ht="15.75" customHeight="1">
       <c r="A118" s="14"/>
@@ -5734,6 +6361,11 @@
       <c r="S118" s="23"/>
       <c r="T118" s="23"/>
       <c r="U118" s="23"/>
+      <c r="V118" s="23"/>
+      <c r="W118" s="23"/>
+      <c r="X118" s="23"/>
+      <c r="Y118" s="23"/>
+      <c r="Z118" s="23"/>
     </row>
     <row r="119" ht="15.75" customHeight="1">
       <c r="A119" s="14"/>
@@ -5757,6 +6389,11 @@
       <c r="S119" s="23"/>
       <c r="T119" s="23"/>
       <c r="U119" s="23"/>
+      <c r="V119" s="23"/>
+      <c r="W119" s="23"/>
+      <c r="X119" s="23"/>
+      <c r="Y119" s="23"/>
+      <c r="Z119" s="23"/>
     </row>
     <row r="120" ht="15.75" customHeight="1">
       <c r="A120" s="14"/>
@@ -5780,6 +6417,11 @@
       <c r="S120" s="23"/>
       <c r="T120" s="23"/>
       <c r="U120" s="23"/>
+      <c r="V120" s="23"/>
+      <c r="W120" s="23"/>
+      <c r="X120" s="23"/>
+      <c r="Y120" s="23"/>
+      <c r="Z120" s="23"/>
     </row>
     <row r="121" ht="15.75" customHeight="1">
       <c r="A121" s="14"/>
@@ -5803,6 +6445,11 @@
       <c r="S121" s="23"/>
       <c r="T121" s="23"/>
       <c r="U121" s="23"/>
+      <c r="V121" s="23"/>
+      <c r="W121" s="23"/>
+      <c r="X121" s="23"/>
+      <c r="Y121" s="23"/>
+      <c r="Z121" s="23"/>
     </row>
     <row r="122" ht="15.75" customHeight="1">
       <c r="A122" s="14"/>
@@ -5826,6 +6473,11 @@
       <c r="S122" s="23"/>
       <c r="T122" s="23"/>
       <c r="U122" s="23"/>
+      <c r="V122" s="23"/>
+      <c r="W122" s="23"/>
+      <c r="X122" s="23"/>
+      <c r="Y122" s="23"/>
+      <c r="Z122" s="23"/>
     </row>
     <row r="123" ht="15.75" customHeight="1">
       <c r="A123" s="14"/>
@@ -5849,6 +6501,11 @@
       <c r="S123" s="23"/>
       <c r="T123" s="23"/>
       <c r="U123" s="23"/>
+      <c r="V123" s="23"/>
+      <c r="W123" s="23"/>
+      <c r="X123" s="23"/>
+      <c r="Y123" s="23"/>
+      <c r="Z123" s="23"/>
     </row>
     <row r="124" ht="15.75" customHeight="1">
       <c r="A124" s="14"/>
@@ -5872,6 +6529,11 @@
       <c r="S124" s="23"/>
       <c r="T124" s="23"/>
       <c r="U124" s="23"/>
+      <c r="V124" s="23"/>
+      <c r="W124" s="23"/>
+      <c r="X124" s="23"/>
+      <c r="Y124" s="23"/>
+      <c r="Z124" s="23"/>
     </row>
     <row r="125" ht="15.75" customHeight="1">
       <c r="A125" s="14"/>
@@ -5895,6 +6557,11 @@
       <c r="S125" s="23"/>
       <c r="T125" s="23"/>
       <c r="U125" s="23"/>
+      <c r="V125" s="23"/>
+      <c r="W125" s="23"/>
+      <c r="X125" s="23"/>
+      <c r="Y125" s="23"/>
+      <c r="Z125" s="23"/>
     </row>
     <row r="126" ht="15.75" customHeight="1">
       <c r="A126" s="14"/>
@@ -5918,6 +6585,11 @@
       <c r="S126" s="23"/>
       <c r="T126" s="23"/>
       <c r="U126" s="23"/>
+      <c r="V126" s="23"/>
+      <c r="W126" s="23"/>
+      <c r="X126" s="23"/>
+      <c r="Y126" s="23"/>
+      <c r="Z126" s="23"/>
     </row>
     <row r="127" ht="15.75" customHeight="1">
       <c r="A127" s="14"/>
@@ -5941,6 +6613,11 @@
       <c r="S127" s="23"/>
       <c r="T127" s="23"/>
       <c r="U127" s="23"/>
+      <c r="V127" s="23"/>
+      <c r="W127" s="23"/>
+      <c r="X127" s="23"/>
+      <c r="Y127" s="23"/>
+      <c r="Z127" s="23"/>
     </row>
     <row r="128" ht="15.75" customHeight="1">
       <c r="A128" s="14"/>
@@ -5964,6 +6641,11 @@
       <c r="S128" s="23"/>
       <c r="T128" s="23"/>
       <c r="U128" s="23"/>
+      <c r="V128" s="23"/>
+      <c r="W128" s="23"/>
+      <c r="X128" s="23"/>
+      <c r="Y128" s="23"/>
+      <c r="Z128" s="23"/>
     </row>
     <row r="129" ht="15.75" customHeight="1">
       <c r="A129" s="14"/>
@@ -5987,6 +6669,11 @@
       <c r="S129" s="23"/>
       <c r="T129" s="23"/>
       <c r="U129" s="23"/>
+      <c r="V129" s="23"/>
+      <c r="W129" s="23"/>
+      <c r="X129" s="23"/>
+      <c r="Y129" s="23"/>
+      <c r="Z129" s="23"/>
     </row>
     <row r="130" ht="15.75" customHeight="1">
       <c r="A130" s="14"/>
@@ -6010,6 +6697,11 @@
       <c r="S130" s="23"/>
       <c r="T130" s="23"/>
       <c r="U130" s="23"/>
+      <c r="V130" s="23"/>
+      <c r="W130" s="23"/>
+      <c r="X130" s="23"/>
+      <c r="Y130" s="23"/>
+      <c r="Z130" s="23"/>
     </row>
     <row r="131" ht="15.75" customHeight="1">
       <c r="A131" s="14"/>
@@ -6033,6 +6725,11 @@
       <c r="S131" s="23"/>
       <c r="T131" s="23"/>
       <c r="U131" s="23"/>
+      <c r="V131" s="23"/>
+      <c r="W131" s="23"/>
+      <c r="X131" s="23"/>
+      <c r="Y131" s="23"/>
+      <c r="Z131" s="23"/>
     </row>
     <row r="132" ht="15.75" customHeight="1">
       <c r="A132" s="14"/>
@@ -6056,6 +6753,11 @@
       <c r="S132" s="23"/>
       <c r="T132" s="23"/>
       <c r="U132" s="23"/>
+      <c r="V132" s="23"/>
+      <c r="W132" s="23"/>
+      <c r="X132" s="23"/>
+      <c r="Y132" s="23"/>
+      <c r="Z132" s="23"/>
     </row>
     <row r="133" ht="15.75" customHeight="1">
       <c r="A133" s="14"/>
@@ -6079,6 +6781,11 @@
       <c r="S133" s="23"/>
       <c r="T133" s="23"/>
       <c r="U133" s="23"/>
+      <c r="V133" s="23"/>
+      <c r="W133" s="23"/>
+      <c r="X133" s="23"/>
+      <c r="Y133" s="23"/>
+      <c r="Z133" s="23"/>
     </row>
     <row r="134" ht="15.75" customHeight="1">
       <c r="A134" s="14"/>
@@ -6102,6 +6809,11 @@
       <c r="S134" s="23"/>
       <c r="T134" s="23"/>
       <c r="U134" s="23"/>
+      <c r="V134" s="23"/>
+      <c r="W134" s="23"/>
+      <c r="X134" s="23"/>
+      <c r="Y134" s="23"/>
+      <c r="Z134" s="23"/>
     </row>
     <row r="135" ht="15.75" customHeight="1">
       <c r="A135" s="14"/>
@@ -6125,6 +6837,11 @@
       <c r="S135" s="23"/>
       <c r="T135" s="23"/>
       <c r="U135" s="23"/>
+      <c r="V135" s="23"/>
+      <c r="W135" s="23"/>
+      <c r="X135" s="23"/>
+      <c r="Y135" s="23"/>
+      <c r="Z135" s="23"/>
     </row>
     <row r="136" ht="15.75" customHeight="1">
       <c r="A136" s="14"/>
@@ -6148,6 +6865,11 @@
       <c r="S136" s="23"/>
       <c r="T136" s="23"/>
       <c r="U136" s="23"/>
+      <c r="V136" s="23"/>
+      <c r="W136" s="23"/>
+      <c r="X136" s="23"/>
+      <c r="Y136" s="23"/>
+      <c r="Z136" s="23"/>
     </row>
     <row r="137" ht="15.75" customHeight="1">
       <c r="A137" s="14"/>
@@ -6171,6 +6893,11 @@
       <c r="S137" s="23"/>
       <c r="T137" s="23"/>
       <c r="U137" s="23"/>
+      <c r="V137" s="23"/>
+      <c r="W137" s="23"/>
+      <c r="X137" s="23"/>
+      <c r="Y137" s="23"/>
+      <c r="Z137" s="23"/>
     </row>
     <row r="138" ht="15.75" customHeight="1">
       <c r="A138" s="14"/>
@@ -6194,6 +6921,11 @@
       <c r="S138" s="23"/>
       <c r="T138" s="23"/>
       <c r="U138" s="23"/>
+      <c r="V138" s="23"/>
+      <c r="W138" s="23"/>
+      <c r="X138" s="23"/>
+      <c r="Y138" s="23"/>
+      <c r="Z138" s="23"/>
     </row>
     <row r="139" ht="15.75" customHeight="1">
       <c r="A139" s="14"/>
@@ -6217,6 +6949,11 @@
       <c r="S139" s="23"/>
       <c r="T139" s="23"/>
       <c r="U139" s="23"/>
+      <c r="V139" s="23"/>
+      <c r="W139" s="23"/>
+      <c r="X139" s="23"/>
+      <c r="Y139" s="23"/>
+      <c r="Z139" s="23"/>
     </row>
     <row r="140" ht="15.75" customHeight="1">
       <c r="A140" s="14"/>
@@ -6240,6 +6977,11 @@
       <c r="S140" s="23"/>
       <c r="T140" s="23"/>
       <c r="U140" s="23"/>
+      <c r="V140" s="23"/>
+      <c r="W140" s="23"/>
+      <c r="X140" s="23"/>
+      <c r="Y140" s="23"/>
+      <c r="Z140" s="23"/>
     </row>
     <row r="141" ht="15.75" customHeight="1">
       <c r="A141" s="14"/>
@@ -6263,6 +7005,11 @@
       <c r="S141" s="23"/>
       <c r="T141" s="23"/>
       <c r="U141" s="23"/>
+      <c r="V141" s="23"/>
+      <c r="W141" s="23"/>
+      <c r="X141" s="23"/>
+      <c r="Y141" s="23"/>
+      <c r="Z141" s="23"/>
     </row>
     <row r="142" ht="15.75" customHeight="1">
       <c r="A142" s="14"/>
@@ -6286,6 +7033,11 @@
       <c r="S142" s="23"/>
       <c r="T142" s="23"/>
       <c r="U142" s="23"/>
+      <c r="V142" s="23"/>
+      <c r="W142" s="23"/>
+      <c r="X142" s="23"/>
+      <c r="Y142" s="23"/>
+      <c r="Z142" s="23"/>
     </row>
     <row r="143" ht="15.75" customHeight="1">
       <c r="A143" s="14"/>
@@ -6309,6 +7061,11 @@
       <c r="S143" s="23"/>
       <c r="T143" s="23"/>
       <c r="U143" s="23"/>
+      <c r="V143" s="23"/>
+      <c r="W143" s="23"/>
+      <c r="X143" s="23"/>
+      <c r="Y143" s="23"/>
+      <c r="Z143" s="23"/>
     </row>
     <row r="144" ht="15.75" customHeight="1">
       <c r="A144" s="14"/>
@@ -6332,6 +7089,11 @@
       <c r="S144" s="23"/>
       <c r="T144" s="23"/>
       <c r="U144" s="23"/>
+      <c r="V144" s="23"/>
+      <c r="W144" s="23"/>
+      <c r="X144" s="23"/>
+      <c r="Y144" s="23"/>
+      <c r="Z144" s="23"/>
     </row>
     <row r="145" ht="15.75" customHeight="1">
       <c r="A145" s="14"/>
@@ -6355,6 +7117,11 @@
       <c r="S145" s="23"/>
       <c r="T145" s="23"/>
       <c r="U145" s="23"/>
+      <c r="V145" s="23"/>
+      <c r="W145" s="23"/>
+      <c r="X145" s="23"/>
+      <c r="Y145" s="23"/>
+      <c r="Z145" s="23"/>
     </row>
     <row r="146" ht="15.75" customHeight="1">
       <c r="A146" s="14"/>
@@ -6378,6 +7145,11 @@
       <c r="S146" s="23"/>
       <c r="T146" s="23"/>
       <c r="U146" s="23"/>
+      <c r="V146" s="23"/>
+      <c r="W146" s="23"/>
+      <c r="X146" s="23"/>
+      <c r="Y146" s="23"/>
+      <c r="Z146" s="23"/>
     </row>
     <row r="147" ht="15.75" customHeight="1">
       <c r="A147" s="14"/>
@@ -6401,6 +7173,11 @@
       <c r="S147" s="23"/>
       <c r="T147" s="23"/>
       <c r="U147" s="23"/>
+      <c r="V147" s="23"/>
+      <c r="W147" s="23"/>
+      <c r="X147" s="23"/>
+      <c r="Y147" s="23"/>
+      <c r="Z147" s="23"/>
     </row>
     <row r="148" ht="15.75" customHeight="1">
       <c r="A148" s="14"/>
@@ -6424,6 +7201,11 @@
       <c r="S148" s="23"/>
       <c r="T148" s="23"/>
       <c r="U148" s="23"/>
+      <c r="V148" s="23"/>
+      <c r="W148" s="23"/>
+      <c r="X148" s="23"/>
+      <c r="Y148" s="23"/>
+      <c r="Z148" s="23"/>
     </row>
     <row r="149" ht="15.75" customHeight="1">
       <c r="A149" s="14"/>
@@ -6447,6 +7229,11 @@
       <c r="S149" s="23"/>
       <c r="T149" s="23"/>
       <c r="U149" s="23"/>
+      <c r="V149" s="23"/>
+      <c r="W149" s="23"/>
+      <c r="X149" s="23"/>
+      <c r="Y149" s="23"/>
+      <c r="Z149" s="23"/>
     </row>
     <row r="150" ht="15.75" customHeight="1">
       <c r="A150" s="14"/>
@@ -6470,6 +7257,11 @@
       <c r="S150" s="23"/>
       <c r="T150" s="23"/>
       <c r="U150" s="23"/>
+      <c r="V150" s="23"/>
+      <c r="W150" s="23"/>
+      <c r="X150" s="23"/>
+      <c r="Y150" s="23"/>
+      <c r="Z150" s="23"/>
     </row>
     <row r="151" ht="15.75" customHeight="1">
       <c r="A151" s="14"/>
@@ -6493,6 +7285,11 @@
       <c r="S151" s="23"/>
       <c r="T151" s="23"/>
       <c r="U151" s="23"/>
+      <c r="V151" s="23"/>
+      <c r="W151" s="23"/>
+      <c r="X151" s="23"/>
+      <c r="Y151" s="23"/>
+      <c r="Z151" s="23"/>
     </row>
     <row r="152" ht="15.75" customHeight="1">
       <c r="A152" s="14"/>
@@ -6516,6 +7313,11 @@
       <c r="S152" s="23"/>
       <c r="T152" s="23"/>
       <c r="U152" s="23"/>
+      <c r="V152" s="23"/>
+      <c r="W152" s="23"/>
+      <c r="X152" s="23"/>
+      <c r="Y152" s="23"/>
+      <c r="Z152" s="23"/>
     </row>
     <row r="153" ht="15.75" customHeight="1">
       <c r="A153" s="14"/>
@@ -6539,6 +7341,11 @@
       <c r="S153" s="23"/>
       <c r="T153" s="23"/>
       <c r="U153" s="23"/>
+      <c r="V153" s="23"/>
+      <c r="W153" s="23"/>
+      <c r="X153" s="23"/>
+      <c r="Y153" s="23"/>
+      <c r="Z153" s="23"/>
     </row>
     <row r="154" ht="15.75" customHeight="1">
       <c r="A154" s="14"/>
@@ -6562,6 +7369,11 @@
       <c r="S154" s="23"/>
       <c r="T154" s="23"/>
       <c r="U154" s="23"/>
+      <c r="V154" s="23"/>
+      <c r="W154" s="23"/>
+      <c r="X154" s="23"/>
+      <c r="Y154" s="23"/>
+      <c r="Z154" s="23"/>
     </row>
     <row r="155" ht="15.75" customHeight="1">
       <c r="A155" s="14"/>
@@ -6585,6 +7397,11 @@
       <c r="S155" s="23"/>
       <c r="T155" s="23"/>
       <c r="U155" s="23"/>
+      <c r="V155" s="23"/>
+      <c r="W155" s="23"/>
+      <c r="X155" s="23"/>
+      <c r="Y155" s="23"/>
+      <c r="Z155" s="23"/>
     </row>
     <row r="156" ht="15.75" customHeight="1">
       <c r="A156" s="14"/>
@@ -6608,6 +7425,11 @@
       <c r="S156" s="23"/>
       <c r="T156" s="23"/>
       <c r="U156" s="23"/>
+      <c r="V156" s="23"/>
+      <c r="W156" s="23"/>
+      <c r="X156" s="23"/>
+      <c r="Y156" s="23"/>
+      <c r="Z156" s="23"/>
     </row>
     <row r="157" ht="15.75" customHeight="1">
       <c r="A157" s="14"/>
@@ -6631,6 +7453,11 @@
       <c r="S157" s="23"/>
       <c r="T157" s="23"/>
       <c r="U157" s="23"/>
+      <c r="V157" s="23"/>
+      <c r="W157" s="23"/>
+      <c r="X157" s="23"/>
+      <c r="Y157" s="23"/>
+      <c r="Z157" s="23"/>
     </row>
     <row r="158" ht="15.75" customHeight="1">
       <c r="A158" s="14"/>
@@ -6654,6 +7481,11 @@
       <c r="S158" s="23"/>
       <c r="T158" s="23"/>
       <c r="U158" s="23"/>
+      <c r="V158" s="23"/>
+      <c r="W158" s="23"/>
+      <c r="X158" s="23"/>
+      <c r="Y158" s="23"/>
+      <c r="Z158" s="23"/>
     </row>
     <row r="159" ht="15.75" customHeight="1">
       <c r="A159" s="14"/>
@@ -6677,6 +7509,11 @@
       <c r="S159" s="23"/>
       <c r="T159" s="23"/>
       <c r="U159" s="23"/>
+      <c r="V159" s="23"/>
+      <c r="W159" s="23"/>
+      <c r="X159" s="23"/>
+      <c r="Y159" s="23"/>
+      <c r="Z159" s="23"/>
     </row>
     <row r="160" ht="15.75" customHeight="1">
       <c r="A160" s="14"/>
@@ -6700,6 +7537,11 @@
       <c r="S160" s="23"/>
       <c r="T160" s="23"/>
       <c r="U160" s="23"/>
+      <c r="V160" s="23"/>
+      <c r="W160" s="23"/>
+      <c r="X160" s="23"/>
+      <c r="Y160" s="23"/>
+      <c r="Z160" s="23"/>
     </row>
     <row r="161" ht="15.75" customHeight="1">
       <c r="A161" s="14"/>
@@ -6723,6 +7565,11 @@
       <c r="S161" s="23"/>
       <c r="T161" s="23"/>
       <c r="U161" s="23"/>
+      <c r="V161" s="23"/>
+      <c r="W161" s="23"/>
+      <c r="X161" s="23"/>
+      <c r="Y161" s="23"/>
+      <c r="Z161" s="23"/>
     </row>
     <row r="162" ht="15.75" customHeight="1">
       <c r="A162" s="14"/>
@@ -6746,6 +7593,11 @@
       <c r="S162" s="23"/>
       <c r="T162" s="23"/>
       <c r="U162" s="23"/>
+      <c r="V162" s="23"/>
+      <c r="W162" s="23"/>
+      <c r="X162" s="23"/>
+      <c r="Y162" s="23"/>
+      <c r="Z162" s="23"/>
     </row>
     <row r="163" ht="15.75" customHeight="1">
       <c r="A163" s="14"/>
@@ -6769,6 +7621,11 @@
       <c r="S163" s="23"/>
       <c r="T163" s="23"/>
       <c r="U163" s="23"/>
+      <c r="V163" s="23"/>
+      <c r="W163" s="23"/>
+      <c r="X163" s="23"/>
+      <c r="Y163" s="23"/>
+      <c r="Z163" s="23"/>
     </row>
     <row r="164" ht="15.75" customHeight="1">
       <c r="A164" s="14"/>
@@ -6792,6 +7649,11 @@
       <c r="S164" s="23"/>
       <c r="T164" s="23"/>
       <c r="U164" s="23"/>
+      <c r="V164" s="23"/>
+      <c r="W164" s="23"/>
+      <c r="X164" s="23"/>
+      <c r="Y164" s="23"/>
+      <c r="Z164" s="23"/>
     </row>
     <row r="165" ht="15.75" customHeight="1">
       <c r="A165" s="14"/>
@@ -6815,6 +7677,11 @@
       <c r="S165" s="23"/>
       <c r="T165" s="23"/>
       <c r="U165" s="23"/>
+      <c r="V165" s="23"/>
+      <c r="W165" s="23"/>
+      <c r="X165" s="23"/>
+      <c r="Y165" s="23"/>
+      <c r="Z165" s="23"/>
     </row>
     <row r="166" ht="15.75" customHeight="1">
       <c r="A166" s="14"/>
@@ -6838,6 +7705,11 @@
       <c r="S166" s="23"/>
       <c r="T166" s="23"/>
       <c r="U166" s="23"/>
+      <c r="V166" s="23"/>
+      <c r="W166" s="23"/>
+      <c r="X166" s="23"/>
+      <c r="Y166" s="23"/>
+      <c r="Z166" s="23"/>
     </row>
     <row r="167" ht="15.75" customHeight="1">
       <c r="A167" s="14"/>
@@ -6861,6 +7733,11 @@
       <c r="S167" s="23"/>
       <c r="T167" s="23"/>
       <c r="U167" s="23"/>
+      <c r="V167" s="23"/>
+      <c r="W167" s="23"/>
+      <c r="X167" s="23"/>
+      <c r="Y167" s="23"/>
+      <c r="Z167" s="23"/>
     </row>
     <row r="168" ht="15.75" customHeight="1">
       <c r="A168" s="14"/>
@@ -6884,6 +7761,11 @@
       <c r="S168" s="23"/>
       <c r="T168" s="23"/>
       <c r="U168" s="23"/>
+      <c r="V168" s="23"/>
+      <c r="W168" s="23"/>
+      <c r="X168" s="23"/>
+      <c r="Y168" s="23"/>
+      <c r="Z168" s="23"/>
     </row>
     <row r="169" ht="15.75" customHeight="1">
       <c r="A169" s="14"/>
@@ -6907,6 +7789,11 @@
       <c r="S169" s="23"/>
       <c r="T169" s="23"/>
       <c r="U169" s="23"/>
+      <c r="V169" s="23"/>
+      <c r="W169" s="23"/>
+      <c r="X169" s="23"/>
+      <c r="Y169" s="23"/>
+      <c r="Z169" s="23"/>
     </row>
     <row r="170" ht="15.75" customHeight="1">
       <c r="A170" s="14"/>
@@ -6930,6 +7817,11 @@
       <c r="S170" s="23"/>
       <c r="T170" s="23"/>
       <c r="U170" s="23"/>
+      <c r="V170" s="23"/>
+      <c r="W170" s="23"/>
+      <c r="X170" s="23"/>
+      <c r="Y170" s="23"/>
+      <c r="Z170" s="23"/>
     </row>
     <row r="171" ht="15.75" customHeight="1">
       <c r="A171" s="14"/>
@@ -6953,6 +7845,11 @@
       <c r="S171" s="23"/>
       <c r="T171" s="23"/>
       <c r="U171" s="23"/>
+      <c r="V171" s="23"/>
+      <c r="W171" s="23"/>
+      <c r="X171" s="23"/>
+      <c r="Y171" s="23"/>
+      <c r="Z171" s="23"/>
     </row>
     <row r="172" ht="15.75" customHeight="1">
       <c r="A172" s="14"/>
@@ -6976,6 +7873,11 @@
       <c r="S172" s="23"/>
       <c r="T172" s="23"/>
       <c r="U172" s="23"/>
+      <c r="V172" s="23"/>
+      <c r="W172" s="23"/>
+      <c r="X172" s="23"/>
+      <c r="Y172" s="23"/>
+      <c r="Z172" s="23"/>
     </row>
     <row r="173" ht="15.75" customHeight="1">
       <c r="A173" s="14"/>
@@ -6999,6 +7901,11 @@
       <c r="S173" s="23"/>
       <c r="T173" s="23"/>
       <c r="U173" s="23"/>
+      <c r="V173" s="23"/>
+      <c r="W173" s="23"/>
+      <c r="X173" s="23"/>
+      <c r="Y173" s="23"/>
+      <c r="Z173" s="23"/>
     </row>
     <row r="174" ht="15.75" customHeight="1">
       <c r="A174" s="14"/>
@@ -7022,6 +7929,11 @@
       <c r="S174" s="23"/>
       <c r="T174" s="23"/>
       <c r="U174" s="23"/>
+      <c r="V174" s="23"/>
+      <c r="W174" s="23"/>
+      <c r="X174" s="23"/>
+      <c r="Y174" s="23"/>
+      <c r="Z174" s="23"/>
     </row>
     <row r="175" ht="15.75" customHeight="1">
       <c r="A175" s="14"/>
@@ -7045,6 +7957,11 @@
       <c r="S175" s="23"/>
       <c r="T175" s="23"/>
       <c r="U175" s="23"/>
+      <c r="V175" s="23"/>
+      <c r="W175" s="23"/>
+      <c r="X175" s="23"/>
+      <c r="Y175" s="23"/>
+      <c r="Z175" s="23"/>
     </row>
     <row r="176" ht="15.75" customHeight="1">
       <c r="A176" s="14"/>
@@ -7068,6 +7985,11 @@
       <c r="S176" s="23"/>
       <c r="T176" s="23"/>
       <c r="U176" s="23"/>
+      <c r="V176" s="23"/>
+      <c r="W176" s="23"/>
+      <c r="X176" s="23"/>
+      <c r="Y176" s="23"/>
+      <c r="Z176" s="23"/>
     </row>
     <row r="177" ht="15.75" customHeight="1">
       <c r="A177" s="14"/>
@@ -7091,6 +8013,11 @@
       <c r="S177" s="23"/>
       <c r="T177" s="23"/>
       <c r="U177" s="23"/>
+      <c r="V177" s="23"/>
+      <c r="W177" s="23"/>
+      <c r="X177" s="23"/>
+      <c r="Y177" s="23"/>
+      <c r="Z177" s="23"/>
     </row>
     <row r="178" ht="15.75" customHeight="1">
       <c r="A178" s="14"/>
@@ -7114,6 +8041,11 @@
       <c r="S178" s="23"/>
       <c r="T178" s="23"/>
       <c r="U178" s="23"/>
+      <c r="V178" s="23"/>
+      <c r="W178" s="23"/>
+      <c r="X178" s="23"/>
+      <c r="Y178" s="23"/>
+      <c r="Z178" s="23"/>
     </row>
     <row r="179" ht="15.75" customHeight="1">
       <c r="A179" s="14"/>
@@ -7137,6 +8069,11 @@
       <c r="S179" s="23"/>
       <c r="T179" s="23"/>
       <c r="U179" s="23"/>
+      <c r="V179" s="23"/>
+      <c r="W179" s="23"/>
+      <c r="X179" s="23"/>
+      <c r="Y179" s="23"/>
+      <c r="Z179" s="23"/>
     </row>
     <row r="180" ht="15.75" customHeight="1">
       <c r="A180" s="14"/>
@@ -7160,6 +8097,11 @@
       <c r="S180" s="23"/>
       <c r="T180" s="23"/>
       <c r="U180" s="23"/>
+      <c r="V180" s="23"/>
+      <c r="W180" s="23"/>
+      <c r="X180" s="23"/>
+      <c r="Y180" s="23"/>
+      <c r="Z180" s="23"/>
     </row>
     <row r="181" ht="15.75" customHeight="1">
       <c r="A181" s="14"/>
@@ -7183,6 +8125,11 @@
       <c r="S181" s="23"/>
       <c r="T181" s="23"/>
       <c r="U181" s="23"/>
+      <c r="V181" s="23"/>
+      <c r="W181" s="23"/>
+      <c r="X181" s="23"/>
+      <c r="Y181" s="23"/>
+      <c r="Z181" s="23"/>
     </row>
     <row r="182" ht="15.75" customHeight="1">
       <c r="A182" s="14"/>
@@ -7206,6 +8153,11 @@
       <c r="S182" s="23"/>
       <c r="T182" s="23"/>
       <c r="U182" s="23"/>
+      <c r="V182" s="23"/>
+      <c r="W182" s="23"/>
+      <c r="X182" s="23"/>
+      <c r="Y182" s="23"/>
+      <c r="Z182" s="23"/>
     </row>
     <row r="183" ht="15.75" customHeight="1">
       <c r="A183" s="14"/>
@@ -7229,6 +8181,11 @@
       <c r="S183" s="23"/>
       <c r="T183" s="23"/>
       <c r="U183" s="23"/>
+      <c r="V183" s="23"/>
+      <c r="W183" s="23"/>
+      <c r="X183" s="23"/>
+      <c r="Y183" s="23"/>
+      <c r="Z183" s="23"/>
     </row>
     <row r="184" ht="15.75" customHeight="1">
       <c r="A184" s="14"/>
@@ -7252,6 +8209,11 @@
       <c r="S184" s="23"/>
       <c r="T184" s="23"/>
       <c r="U184" s="23"/>
+      <c r="V184" s="23"/>
+      <c r="W184" s="23"/>
+      <c r="X184" s="23"/>
+      <c r="Y184" s="23"/>
+      <c r="Z184" s="23"/>
     </row>
     <row r="185" ht="15.75" customHeight="1">
       <c r="A185" s="14"/>
@@ -7275,6 +8237,11 @@
       <c r="S185" s="23"/>
       <c r="T185" s="23"/>
       <c r="U185" s="23"/>
+      <c r="V185" s="23"/>
+      <c r="W185" s="23"/>
+      <c r="X185" s="23"/>
+      <c r="Y185" s="23"/>
+      <c r="Z185" s="23"/>
     </row>
     <row r="186" ht="15.75" customHeight="1">
       <c r="A186" s="14"/>
@@ -7298,6 +8265,11 @@
       <c r="S186" s="23"/>
       <c r="T186" s="23"/>
       <c r="U186" s="23"/>
+      <c r="V186" s="23"/>
+      <c r="W186" s="23"/>
+      <c r="X186" s="23"/>
+      <c r="Y186" s="23"/>
+      <c r="Z186" s="23"/>
     </row>
     <row r="187" ht="15.75" customHeight="1">
       <c r="A187" s="14"/>
@@ -7321,6 +8293,11 @@
       <c r="S187" s="23"/>
       <c r="T187" s="23"/>
       <c r="U187" s="23"/>
+      <c r="V187" s="23"/>
+      <c r="W187" s="23"/>
+      <c r="X187" s="23"/>
+      <c r="Y187" s="23"/>
+      <c r="Z187" s="23"/>
     </row>
     <row r="188" ht="15.75" customHeight="1">
       <c r="A188" s="14"/>
@@ -7344,6 +8321,11 @@
       <c r="S188" s="23"/>
       <c r="T188" s="23"/>
       <c r="U188" s="23"/>
+      <c r="V188" s="23"/>
+      <c r="W188" s="23"/>
+      <c r="X188" s="23"/>
+      <c r="Y188" s="23"/>
+      <c r="Z188" s="23"/>
     </row>
     <row r="189" ht="15.75" customHeight="1">
       <c r="A189" s="14"/>
@@ -7367,6 +8349,11 @@
       <c r="S189" s="23"/>
       <c r="T189" s="23"/>
       <c r="U189" s="23"/>
+      <c r="V189" s="23"/>
+      <c r="W189" s="23"/>
+      <c r="X189" s="23"/>
+      <c r="Y189" s="23"/>
+      <c r="Z189" s="23"/>
     </row>
     <row r="190" ht="15.75" customHeight="1">
       <c r="A190" s="14"/>
@@ -7390,6 +8377,11 @@
       <c r="S190" s="23"/>
       <c r="T190" s="23"/>
       <c r="U190" s="23"/>
+      <c r="V190" s="23"/>
+      <c r="W190" s="23"/>
+      <c r="X190" s="23"/>
+      <c r="Y190" s="23"/>
+      <c r="Z190" s="23"/>
     </row>
     <row r="191" ht="15.75" customHeight="1">
       <c r="A191" s="14"/>
@@ -7413,6 +8405,11 @@
       <c r="S191" s="23"/>
       <c r="T191" s="23"/>
       <c r="U191" s="23"/>
+      <c r="V191" s="23"/>
+      <c r="W191" s="23"/>
+      <c r="X191" s="23"/>
+      <c r="Y191" s="23"/>
+      <c r="Z191" s="23"/>
     </row>
     <row r="192" ht="15.75" customHeight="1">
       <c r="A192" s="14"/>
@@ -7436,6 +8433,11 @@
       <c r="S192" s="23"/>
       <c r="T192" s="23"/>
       <c r="U192" s="23"/>
+      <c r="V192" s="23"/>
+      <c r="W192" s="23"/>
+      <c r="X192" s="23"/>
+      <c r="Y192" s="23"/>
+      <c r="Z192" s="23"/>
     </row>
     <row r="193" ht="15.75" customHeight="1">
       <c r="A193" s="14"/>
@@ -7459,6 +8461,11 @@
       <c r="S193" s="23"/>
       <c r="T193" s="23"/>
       <c r="U193" s="23"/>
+      <c r="V193" s="23"/>
+      <c r="W193" s="23"/>
+      <c r="X193" s="23"/>
+      <c r="Y193" s="23"/>
+      <c r="Z193" s="23"/>
     </row>
     <row r="194" ht="15.75" customHeight="1">
       <c r="A194" s="14"/>
@@ -7482,6 +8489,11 @@
       <c r="S194" s="23"/>
       <c r="T194" s="23"/>
       <c r="U194" s="23"/>
+      <c r="V194" s="23"/>
+      <c r="W194" s="23"/>
+      <c r="X194" s="23"/>
+      <c r="Y194" s="23"/>
+      <c r="Z194" s="23"/>
     </row>
     <row r="195" ht="15.75" customHeight="1">
       <c r="A195" s="14"/>
@@ -7505,6 +8517,11 @@
       <c r="S195" s="23"/>
       <c r="T195" s="23"/>
       <c r="U195" s="23"/>
+      <c r="V195" s="23"/>
+      <c r="W195" s="23"/>
+      <c r="X195" s="23"/>
+      <c r="Y195" s="23"/>
+      <c r="Z195" s="23"/>
     </row>
     <row r="196" ht="15.75" customHeight="1">
       <c r="A196" s="14"/>
@@ -7528,6 +8545,11 @@
       <c r="S196" s="23"/>
       <c r="T196" s="23"/>
       <c r="U196" s="23"/>
+      <c r="V196" s="23"/>
+      <c r="W196" s="23"/>
+      <c r="X196" s="23"/>
+      <c r="Y196" s="23"/>
+      <c r="Z196" s="23"/>
     </row>
     <row r="197" ht="15.75" customHeight="1">
       <c r="A197" s="14"/>
@@ -7551,6 +8573,11 @@
       <c r="S197" s="23"/>
       <c r="T197" s="23"/>
       <c r="U197" s="23"/>
+      <c r="V197" s="23"/>
+      <c r="W197" s="23"/>
+      <c r="X197" s="23"/>
+      <c r="Y197" s="23"/>
+      <c r="Z197" s="23"/>
     </row>
     <row r="198" ht="15.75" customHeight="1">
       <c r="A198" s="14"/>
@@ -7574,6 +8601,11 @@
       <c r="S198" s="23"/>
       <c r="T198" s="23"/>
       <c r="U198" s="23"/>
+      <c r="V198" s="23"/>
+      <c r="W198" s="23"/>
+      <c r="X198" s="23"/>
+      <c r="Y198" s="23"/>
+      <c r="Z198" s="23"/>
     </row>
     <row r="199" ht="15.75" customHeight="1">
       <c r="A199" s="14"/>
@@ -7597,6 +8629,11 @@
       <c r="S199" s="23"/>
       <c r="T199" s="23"/>
       <c r="U199" s="23"/>
+      <c r="V199" s="23"/>
+      <c r="W199" s="23"/>
+      <c r="X199" s="23"/>
+      <c r="Y199" s="23"/>
+      <c r="Z199" s="23"/>
     </row>
     <row r="200" ht="15.75" customHeight="1">
       <c r="A200" s="14"/>
@@ -7620,6 +8657,11 @@
       <c r="S200" s="23"/>
       <c r="T200" s="23"/>
       <c r="U200" s="23"/>
+      <c r="V200" s="23"/>
+      <c r="W200" s="23"/>
+      <c r="X200" s="23"/>
+      <c r="Y200" s="23"/>
+      <c r="Z200" s="23"/>
     </row>
     <row r="201" ht="15.75" customHeight="1">
       <c r="A201" s="14"/>
@@ -7643,6 +8685,11 @@
       <c r="S201" s="23"/>
       <c r="T201" s="23"/>
       <c r="U201" s="23"/>
+      <c r="V201" s="23"/>
+      <c r="W201" s="23"/>
+      <c r="X201" s="23"/>
+      <c r="Y201" s="23"/>
+      <c r="Z201" s="23"/>
     </row>
     <row r="202" ht="15.75" customHeight="1">
       <c r="A202" s="14"/>
@@ -7666,6 +8713,11 @@
       <c r="S202" s="23"/>
       <c r="T202" s="23"/>
       <c r="U202" s="23"/>
+      <c r="V202" s="23"/>
+      <c r="W202" s="23"/>
+      <c r="X202" s="23"/>
+      <c r="Y202" s="23"/>
+      <c r="Z202" s="23"/>
     </row>
     <row r="203" ht="15.75" customHeight="1">
       <c r="A203" s="14"/>
@@ -7689,6 +8741,11 @@
       <c r="S203" s="23"/>
       <c r="T203" s="23"/>
       <c r="U203" s="23"/>
+      <c r="V203" s="23"/>
+      <c r="W203" s="23"/>
+      <c r="X203" s="23"/>
+      <c r="Y203" s="23"/>
+      <c r="Z203" s="23"/>
     </row>
     <row r="204" ht="15.75" customHeight="1">
       <c r="A204" s="14"/>
@@ -7712,6 +8769,11 @@
       <c r="S204" s="23"/>
       <c r="T204" s="23"/>
       <c r="U204" s="23"/>
+      <c r="V204" s="23"/>
+      <c r="W204" s="23"/>
+      <c r="X204" s="23"/>
+      <c r="Y204" s="23"/>
+      <c r="Z204" s="23"/>
     </row>
     <row r="205" ht="15.75" customHeight="1">
       <c r="A205" s="14"/>
@@ -7735,6 +8797,11 @@
       <c r="S205" s="23"/>
       <c r="T205" s="23"/>
       <c r="U205" s="23"/>
+      <c r="V205" s="23"/>
+      <c r="W205" s="23"/>
+      <c r="X205" s="23"/>
+      <c r="Y205" s="23"/>
+      <c r="Z205" s="23"/>
     </row>
     <row r="206" ht="15.75" customHeight="1">
       <c r="A206" s="14"/>
@@ -7758,6 +8825,11 @@
       <c r="S206" s="23"/>
       <c r="T206" s="23"/>
       <c r="U206" s="23"/>
+      <c r="V206" s="23"/>
+      <c r="W206" s="23"/>
+      <c r="X206" s="23"/>
+      <c r="Y206" s="23"/>
+      <c r="Z206" s="23"/>
     </row>
     <row r="207" ht="15.75" customHeight="1">
       <c r="A207" s="14"/>
@@ -7781,6 +8853,11 @@
       <c r="S207" s="23"/>
       <c r="T207" s="23"/>
       <c r="U207" s="23"/>
+      <c r="V207" s="23"/>
+      <c r="W207" s="23"/>
+      <c r="X207" s="23"/>
+      <c r="Y207" s="23"/>
+      <c r="Z207" s="23"/>
     </row>
     <row r="208" ht="15.75" customHeight="1">
       <c r="A208" s="14"/>
@@ -7804,6 +8881,11 @@
       <c r="S208" s="23"/>
       <c r="T208" s="23"/>
       <c r="U208" s="23"/>
+      <c r="V208" s="23"/>
+      <c r="W208" s="23"/>
+      <c r="X208" s="23"/>
+      <c r="Y208" s="23"/>
+      <c r="Z208" s="23"/>
     </row>
     <row r="209" ht="15.75" customHeight="1">
       <c r="A209" s="14"/>
@@ -7827,6 +8909,11 @@
       <c r="S209" s="23"/>
       <c r="T209" s="23"/>
       <c r="U209" s="23"/>
+      <c r="V209" s="23"/>
+      <c r="W209" s="23"/>
+      <c r="X209" s="23"/>
+      <c r="Y209" s="23"/>
+      <c r="Z209" s="23"/>
     </row>
     <row r="210" ht="15.75" customHeight="1">
       <c r="A210" s="14"/>
@@ -7850,6 +8937,11 @@
       <c r="S210" s="23"/>
       <c r="T210" s="23"/>
       <c r="U210" s="23"/>
+      <c r="V210" s="23"/>
+      <c r="W210" s="23"/>
+      <c r="X210" s="23"/>
+      <c r="Y210" s="23"/>
+      <c r="Z210" s="23"/>
     </row>
     <row r="211" ht="15.75" customHeight="1">
       <c r="A211" s="14"/>
@@ -7873,6 +8965,11 @@
       <c r="S211" s="23"/>
       <c r="T211" s="23"/>
       <c r="U211" s="23"/>
+      <c r="V211" s="23"/>
+      <c r="W211" s="23"/>
+      <c r="X211" s="23"/>
+      <c r="Y211" s="23"/>
+      <c r="Z211" s="23"/>
     </row>
     <row r="212" ht="15.75" customHeight="1">
       <c r="A212" s="14"/>
@@ -7896,6 +8993,11 @@
       <c r="S212" s="23"/>
       <c r="T212" s="23"/>
       <c r="U212" s="23"/>
+      <c r="V212" s="23"/>
+      <c r="W212" s="23"/>
+      <c r="X212" s="23"/>
+      <c r="Y212" s="23"/>
+      <c r="Z212" s="23"/>
     </row>
     <row r="213" ht="15.75" customHeight="1">
       <c r="A213" s="14"/>
@@ -7919,6 +9021,11 @@
       <c r="S213" s="23"/>
       <c r="T213" s="23"/>
       <c r="U213" s="23"/>
+      <c r="V213" s="23"/>
+      <c r="W213" s="23"/>
+      <c r="X213" s="23"/>
+      <c r="Y213" s="23"/>
+      <c r="Z213" s="23"/>
     </row>
     <row r="214" ht="15.75" customHeight="1">
       <c r="A214" s="14"/>
@@ -7942,6 +9049,11 @@
       <c r="S214" s="23"/>
       <c r="T214" s="23"/>
       <c r="U214" s="23"/>
+      <c r="V214" s="23"/>
+      <c r="W214" s="23"/>
+      <c r="X214" s="23"/>
+      <c r="Y214" s="23"/>
+      <c r="Z214" s="23"/>
     </row>
     <row r="215" ht="15.75" customHeight="1">
       <c r="A215" s="14"/>
@@ -7965,6 +9077,11 @@
       <c r="S215" s="23"/>
       <c r="T215" s="23"/>
       <c r="U215" s="23"/>
+      <c r="V215" s="23"/>
+      <c r="W215" s="23"/>
+      <c r="X215" s="23"/>
+      <c r="Y215" s="23"/>
+      <c r="Z215" s="23"/>
     </row>
     <row r="216" ht="15.75" customHeight="1">
       <c r="A216" s="14"/>
@@ -7988,6 +9105,11 @@
       <c r="S216" s="23"/>
       <c r="T216" s="23"/>
       <c r="U216" s="23"/>
+      <c r="V216" s="23"/>
+      <c r="W216" s="23"/>
+      <c r="X216" s="23"/>
+      <c r="Y216" s="23"/>
+      <c r="Z216" s="23"/>
     </row>
     <row r="217" ht="15.75" customHeight="1">
       <c r="A217" s="14"/>
@@ -8011,6 +9133,11 @@
       <c r="S217" s="23"/>
       <c r="T217" s="23"/>
       <c r="U217" s="23"/>
+      <c r="V217" s="23"/>
+      <c r="W217" s="23"/>
+      <c r="X217" s="23"/>
+      <c r="Y217" s="23"/>
+      <c r="Z217" s="23"/>
     </row>
     <row r="218" ht="15.75" customHeight="1">
       <c r="A218" s="14"/>
@@ -8034,6 +9161,11 @@
       <c r="S218" s="23"/>
       <c r="T218" s="23"/>
       <c r="U218" s="23"/>
+      <c r="V218" s="23"/>
+      <c r="W218" s="23"/>
+      <c r="X218" s="23"/>
+      <c r="Y218" s="23"/>
+      <c r="Z218" s="23"/>
     </row>
     <row r="219" ht="15.75" customHeight="1">
       <c r="A219" s="14"/>
@@ -8057,6 +9189,11 @@
       <c r="S219" s="23"/>
       <c r="T219" s="23"/>
       <c r="U219" s="23"/>
+      <c r="V219" s="23"/>
+      <c r="W219" s="23"/>
+      <c r="X219" s="23"/>
+      <c r="Y219" s="23"/>
+      <c r="Z219" s="23"/>
     </row>
     <row r="220" ht="15.75" customHeight="1">
       <c r="A220" s="14"/>
@@ -8080,6 +9217,11 @@
       <c r="S220" s="23"/>
       <c r="T220" s="23"/>
       <c r="U220" s="23"/>
+      <c r="V220" s="23"/>
+      <c r="W220" s="23"/>
+      <c r="X220" s="23"/>
+      <c r="Y220" s="23"/>
+      <c r="Z220" s="23"/>
     </row>
     <row r="221" ht="15.75" customHeight="1">
       <c r="A221" s="22"/>
@@ -11202,7 +12344,7 @@
       <c r="C1000" s="22"/>
     </row>
   </sheetData>
-  <autoFilter ref="$A$1:$U$1"/>
+  <autoFilter ref="$A$1:$Z$1"/>
   <dataValidations>
     <dataValidation type="custom" allowBlank="1" showErrorMessage="1" sqref="C2:C1000">
       <formula1>AND(GTE(LEN(C2),MIN((0),(125))),LTE(LEN(C2),MAX((0),(125))))</formula1>
@@ -11240,207 +12382,207 @@
         <v>8</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" s="26" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="26" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="C5" s="27" t="s">
-        <v>49</v>
+        <v>53</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" s="26" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="26" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="26" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="26" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" s="26" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" s="26" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" s="26" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="C12" s="26" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" s="26" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" s="26" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="C14" s="26" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" s="26" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="C15" s="26" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" s="26" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="C16" s="26" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" s="26" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="C17" s="26" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" s="26" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C18" s="26" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" s="26" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C19" s="26" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" s="26" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="C20" s="26" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="B21" s="26" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="C21" s="26" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="B22" s="26" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C22" s="26" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" ht="15.0" customHeight="1">
       <c r="B23" s="26" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="C23" s="26" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" ht="15.0" customHeight="1">
       <c r="B24" s="26" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="C24" s="26" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" ht="15.0" customHeight="1">
       <c r="B25" s="26" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="C25" s="26" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" ht="15.0" customHeight="1">
       <c r="B26" s="26" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="C26" s="26" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="B27" s="26" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="C27" s="26" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
@@ -11450,432 +12592,432 @@
       <c r="B29" s="14"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="B30" s="28" t="s">
+      <c r="B30" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="C30" s="28" t="s">
+      <c r="C30" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="D30" s="28" t="s">
-        <v>43</v>
+      <c r="D30" s="29" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="B31" s="26" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="C31" s="26" t="s">
-        <v>93</v>
-      </c>
-      <c r="D31" s="29" t="s">
-        <v>94</v>
+        <v>98</v>
+      </c>
+      <c r="D31" s="30" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="B32" s="26" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="C32" s="26" t="s">
-        <v>96</v>
-      </c>
-      <c r="D32" s="29" t="s">
-        <v>94</v>
+        <v>101</v>
+      </c>
+      <c r="D32" s="30" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="B33" s="26" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="C33" s="26" t="s">
-        <v>98</v>
-      </c>
-      <c r="D33" s="29" t="s">
-        <v>94</v>
+        <v>103</v>
+      </c>
+      <c r="D33" s="30" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="B34" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="C34" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="D34" s="30" t="s">
         <v>99</v>
-      </c>
-      <c r="C34" s="26" t="s">
-        <v>100</v>
-      </c>
-      <c r="D34" s="29" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="B35" s="26" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="C35" s="26" t="s">
-        <v>102</v>
-      </c>
-      <c r="D35" s="29" t="s">
-        <v>94</v>
+        <v>107</v>
+      </c>
+      <c r="D35" s="30" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="B36" s="26" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="C36" s="26" t="s">
-        <v>104</v>
-      </c>
-      <c r="D36" s="29" t="s">
-        <v>94</v>
+        <v>109</v>
+      </c>
+      <c r="D36" s="30" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="B37" s="26" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="C37" s="26" t="s">
-        <v>106</v>
-      </c>
-      <c r="D37" s="29" t="s">
-        <v>107</v>
+        <v>111</v>
+      </c>
+      <c r="D37" s="30" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="B38" s="26" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="C38" s="26" t="s">
-        <v>109</v>
-      </c>
-      <c r="D38" s="29" t="s">
-        <v>110</v>
+        <v>114</v>
+      </c>
+      <c r="D38" s="30" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="B39" s="26" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="C39" s="26" t="s">
-        <v>112</v>
-      </c>
-      <c r="D39" s="29" t="s">
-        <v>113</v>
+        <v>117</v>
+      </c>
+      <c r="D39" s="30" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="B40" s="26" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="C40" s="26" t="s">
-        <v>115</v>
-      </c>
-      <c r="D40" s="29" t="s">
-        <v>116</v>
+        <v>120</v>
+      </c>
+      <c r="D40" s="30" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="B41" s="26" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="C41" s="26" t="s">
-        <v>118</v>
-      </c>
-      <c r="D41" s="29" t="s">
-        <v>119</v>
+        <v>123</v>
+      </c>
+      <c r="D41" s="30" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="B42" s="26" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="C42" s="26" t="s">
-        <v>121</v>
-      </c>
-      <c r="D42" s="29" t="s">
-        <v>122</v>
+        <v>126</v>
+      </c>
+      <c r="D42" s="30" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="B43" s="26" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="C43" s="26" t="s">
-        <v>124</v>
-      </c>
-      <c r="D43" s="29" t="s">
-        <v>125</v>
+        <v>129</v>
+      </c>
+      <c r="D43" s="30" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="B44" s="26" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="C44" s="26" t="s">
-        <v>127</v>
-      </c>
-      <c r="D44" s="29" t="s">
-        <v>128</v>
+        <v>132</v>
+      </c>
+      <c r="D44" s="30" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="B45" s="26" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="C45" s="26" t="s">
-        <v>130</v>
-      </c>
-      <c r="D45" s="29" t="s">
-        <v>131</v>
+        <v>135</v>
+      </c>
+      <c r="D45" s="30" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="B46" s="26" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="C46" s="26" t="s">
-        <v>133</v>
-      </c>
-      <c r="D46" s="29" t="s">
-        <v>134</v>
+        <v>138</v>
+      </c>
+      <c r="D46" s="30" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="47" ht="15.75" customHeight="1">
       <c r="B47" s="26" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="C47" s="26" t="s">
-        <v>136</v>
-      </c>
-      <c r="D47" s="29" t="s">
-        <v>137</v>
+        <v>141</v>
+      </c>
+      <c r="D47" s="30" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="B48" s="26" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="C48" s="26" t="s">
-        <v>139</v>
-      </c>
-      <c r="D48" s="29" t="s">
-        <v>140</v>
+        <v>144</v>
+      </c>
+      <c r="D48" s="30" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="B49" s="26" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="C49" s="26" t="s">
-        <v>142</v>
-      </c>
-      <c r="D49" s="29" t="s">
-        <v>143</v>
+        <v>147</v>
+      </c>
+      <c r="D49" s="30" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="50" ht="15.75" customHeight="1">
       <c r="B50" s="26" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="C50" s="26" t="s">
-        <v>145</v>
-      </c>
-      <c r="D50" s="29" t="s">
-        <v>146</v>
+        <v>150</v>
+      </c>
+      <c r="D50" s="30" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="51" ht="15.75" customHeight="1">
       <c r="B51" s="26" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="C51" s="26" t="s">
-        <v>148</v>
-      </c>
-      <c r="D51" s="29" t="s">
-        <v>149</v>
+        <v>153</v>
+      </c>
+      <c r="D51" s="30" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="B52" s="26" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C52" s="26" t="s">
-        <v>151</v>
-      </c>
-      <c r="D52" s="29" t="s">
-        <v>152</v>
+        <v>156</v>
+      </c>
+      <c r="D52" s="30" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="B53" s="26" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="C53" s="26" t="s">
-        <v>154</v>
-      </c>
-      <c r="D53" s="29" t="s">
-        <v>155</v>
+        <v>159</v>
+      </c>
+      <c r="D53" s="30" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="B54" s="29" t="s">
-        <v>156</v>
-      </c>
-      <c r="C54" s="29" t="s">
-        <v>157</v>
-      </c>
-      <c r="D54" s="29" t="s">
-        <v>158</v>
+      <c r="B54" s="30" t="s">
+        <v>161</v>
+      </c>
+      <c r="C54" s="30" t="s">
+        <v>162</v>
+      </c>
+      <c r="D54" s="30" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="B55" s="29" t="s">
-        <v>159</v>
-      </c>
-      <c r="C55" s="29" t="s">
-        <v>160</v>
-      </c>
-      <c r="D55" s="29" t="s">
-        <v>161</v>
+      <c r="B55" s="30" t="s">
+        <v>164</v>
+      </c>
+      <c r="C55" s="30" t="s">
+        <v>165</v>
+      </c>
+      <c r="D55" s="30" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="B56" s="29" t="s">
-        <v>162</v>
-      </c>
-      <c r="C56" s="29" t="s">
+      <c r="B56" s="30" t="s">
+        <v>167</v>
+      </c>
+      <c r="C56" s="30" t="s">
+        <v>168</v>
+      </c>
+      <c r="D56" s="30" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="57" ht="15.75" customHeight="1">
+      <c r="B57" s="30" t="s">
+        <v>170</v>
+      </c>
+      <c r="C57" s="30" t="s">
+        <v>171</v>
+      </c>
+      <c r="D57" s="30" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="58" ht="15.75" customHeight="1">
+      <c r="B58" s="30" t="s">
+        <v>173</v>
+      </c>
+      <c r="C58" s="30" t="s">
+        <v>174</v>
+      </c>
+      <c r="D58" s="30" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="59" ht="15.75" customHeight="1">
+      <c r="B59" s="30" t="s">
+        <v>176</v>
+      </c>
+      <c r="C59" s="30" t="s">
+        <v>177</v>
+      </c>
+      <c r="D59" s="30" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="60" ht="15.75" customHeight="1">
+      <c r="B60" s="30" t="s">
+        <v>179</v>
+      </c>
+      <c r="C60" s="30" t="s">
+        <v>180</v>
+      </c>
+      <c r="D60" s="30" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="61" ht="15.75" customHeight="1">
+      <c r="B61" s="30" t="s">
+        <v>182</v>
+      </c>
+      <c r="C61" s="30" t="s">
+        <v>183</v>
+      </c>
+      <c r="D61" s="30" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="62" ht="15.75" customHeight="1">
+      <c r="B62" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="C62" s="30" t="s">
+        <v>186</v>
+      </c>
+      <c r="D62" s="30" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="63" ht="15.75" customHeight="1">
+      <c r="B63" s="30" t="s">
+        <v>188</v>
+      </c>
+      <c r="C63" s="30" t="s">
+        <v>189</v>
+      </c>
+      <c r="D63" s="30" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="64" ht="15.75" customHeight="1">
+      <c r="B64" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="C64" s="30" t="s">
+        <v>192</v>
+      </c>
+      <c r="D64" s="30" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="65" ht="15.75" customHeight="1">
+      <c r="B65" s="30" t="s">
+        <v>194</v>
+      </c>
+      <c r="C65" s="30" t="s">
+        <v>195</v>
+      </c>
+      <c r="D65" s="30" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="66" ht="15.75" customHeight="1">
+      <c r="B66" s="30" t="s">
+        <v>197</v>
+      </c>
+      <c r="C66" s="30" t="s">
+        <v>198</v>
+      </c>
+      <c r="D66" s="30" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="67" ht="15.75" customHeight="1">
+      <c r="B67" s="30" t="s">
+        <v>200</v>
+      </c>
+      <c r="C67" s="30" t="s">
+        <v>201</v>
+      </c>
+      <c r="D67" s="30" t="s">
         <v>163</v>
       </c>
-      <c r="D56" s="29" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="57" ht="15.75" customHeight="1">
-      <c r="B57" s="29" t="s">
-        <v>165</v>
-      </c>
-      <c r="C57" s="29" t="s">
-        <v>166</v>
-      </c>
-      <c r="D57" s="29" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="58" ht="15.75" customHeight="1">
-      <c r="B58" s="29" t="s">
-        <v>168</v>
-      </c>
-      <c r="C58" s="29" t="s">
-        <v>169</v>
-      </c>
-      <c r="D58" s="29" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="59" ht="15.75" customHeight="1">
-      <c r="B59" s="29" t="s">
-        <v>171</v>
-      </c>
-      <c r="C59" s="29" t="s">
-        <v>172</v>
-      </c>
-      <c r="D59" s="29" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="60" ht="15.75" customHeight="1">
-      <c r="B60" s="29" t="s">
-        <v>174</v>
-      </c>
-      <c r="C60" s="29" t="s">
-        <v>175</v>
-      </c>
-      <c r="D60" s="29" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="61" ht="15.75" customHeight="1">
-      <c r="B61" s="29" t="s">
-        <v>177</v>
-      </c>
-      <c r="C61" s="29" t="s">
-        <v>178</v>
-      </c>
-      <c r="D61" s="29" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="62" ht="15.75" customHeight="1">
-      <c r="B62" s="29" t="s">
-        <v>180</v>
-      </c>
-      <c r="C62" s="29" t="s">
-        <v>181</v>
-      </c>
-      <c r="D62" s="29" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="63" ht="15.75" customHeight="1">
-      <c r="B63" s="29" t="s">
-        <v>183</v>
-      </c>
-      <c r="C63" s="29" t="s">
-        <v>184</v>
-      </c>
-      <c r="D63" s="29" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="64" ht="15.75" customHeight="1">
-      <c r="B64" s="29" t="s">
-        <v>186</v>
-      </c>
-      <c r="C64" s="29" t="s">
-        <v>187</v>
-      </c>
-      <c r="D64" s="29" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="65" ht="15.75" customHeight="1">
-      <c r="B65" s="29" t="s">
-        <v>189</v>
-      </c>
-      <c r="C65" s="29" t="s">
-        <v>190</v>
-      </c>
-      <c r="D65" s="29" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="66" ht="15.75" customHeight="1">
-      <c r="B66" s="29" t="s">
-        <v>192</v>
-      </c>
-      <c r="C66" s="29" t="s">
-        <v>193</v>
-      </c>
-      <c r="D66" s="29" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="67" ht="15.75" customHeight="1">
-      <c r="B67" s="29" t="s">
-        <v>195</v>
-      </c>
-      <c r="C67" s="29" t="s">
-        <v>196</v>
-      </c>
-      <c r="D67" s="29" t="s">
-        <v>158</v>
-      </c>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="B68" s="29" t="s">
-        <v>197</v>
-      </c>
-      <c r="C68" s="29" t="s">
-        <v>198</v>
-      </c>
-      <c r="D68" s="29" t="s">
-        <v>107</v>
+      <c r="B68" s="30" t="s">
+        <v>202</v>
+      </c>
+      <c r="C68" s="30" t="s">
+        <v>203</v>
+      </c>
+      <c r="D68" s="30" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="69" ht="15.75" customHeight="1"/>
@@ -12836,46 +13978,52 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="30" t="s">
-        <v>199</v>
-      </c>
-      <c r="B1" s="30" t="s">
-        <v>200</v>
-      </c>
-      <c r="C1" s="30" t="s">
-        <v>201</v>
+      <c r="A1" s="31" t="s">
+        <v>204</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>205</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="31" t="s">
-        <v>202</v>
-      </c>
-      <c r="B2" s="31" t="s">
-        <v>203</v>
-      </c>
-      <c r="C2" s="31" t="s">
-        <v>204</v>
+      <c r="A2" s="32" t="s">
+        <v>207</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>208</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="31"/>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
+      <c r="A3" s="33" t="s">
+        <v>210</v>
+      </c>
+      <c r="B3" s="33" t="s">
+        <v>208</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="31"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
+      <c r="A4" s="32"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
     </row>
     <row r="5">
-      <c r="A5" s="31"/>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
+      <c r="A5" s="32"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
     </row>
     <row r="6">
-      <c r="A6" s="31"/>
-      <c r="B6" s="31"/>
-      <c r="C6" s="31"/>
+      <c r="A6" s="32"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
     </row>
     <row r="7"/>
     <row r="8"/>

</xml_diff>